<commit_message>
updates to try get working structural model
</commit_message>
<xml_diff>
--- a/Data/Data_geology/Otorowiri_outcrop.xlsx
+++ b/Data/Data_geology/Otorowiri_outcrop.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\00105010\Projects\Otorowiri\data\data_geology\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA37F1B3-277F-483C-8B00-4E09CD909D9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9966DA22-6EDC-4940-B65C-745017A8DD0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="3" activeTab="4" xr2:uid="{3885F5B0-7C21-4634-A104-1A3CDF95EC0E}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="4" xr2:uid="{3885F5B0-7C21-4634-A104-1A3CDF95EC0E}"/>
   </bookViews>
   <sheets>
     <sheet name="Otorowiri_1" sheetId="1" r:id="rId1"/>
     <sheet name="Otorowiri_2" sheetId="2" r:id="rId2"/>
     <sheet name="Otorowiri_3" sheetId="3" r:id="rId3"/>
     <sheet name="Otorowiri-Parmelia contact" sheetId="4" r:id="rId4"/>
-    <sheet name="Yarragadee-Otorowiri_NEW" sheetId="6" r:id="rId5"/>
-    <sheet name="Otorowiri-Parmelia_NEW" sheetId="5" r:id="rId6"/>
+    <sheet name="Yarragadee-Otorowiri contact" sheetId="7" r:id="rId5"/>
+    <sheet name="Yarragadee-Otorowiri_NEW" sheetId="6" r:id="rId6"/>
+    <sheet name="Otorowiri-Parmelia_NEW" sheetId="5" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="629">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="629">
   <si>
     <t>Longitude</t>
   </si>
@@ -14726,7 +14727,7 @@
   <dimension ref="A1:D458"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J434" sqref="J434"/>
+      <selection activeCell="D1" sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -21152,11 +21153,3120 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1556757B-BEF5-4EA2-92E7-842579201367}">
+  <dimension ref="A1:D221"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>115.44903107899999</v>
+      </c>
+      <c r="B2">
+        <v>-29.946426558999899</v>
+      </c>
+      <c r="C2">
+        <v>350323.11707107548</v>
+      </c>
+      <c r="D2">
+        <v>6686139.57207515</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>115.447738706</v>
+      </c>
+      <c r="B3">
+        <v>-29.937659003999901</v>
+      </c>
+      <c r="C3">
+        <v>350185.23797649564</v>
+      </c>
+      <c r="D3">
+        <v>6687109.5732190665</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>115.446912842</v>
+      </c>
+      <c r="B4">
+        <v>-29.930629304999901</v>
+      </c>
+      <c r="C4">
+        <v>350094.9800640571</v>
+      </c>
+      <c r="D4">
+        <v>6687887.5793880057</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>115.446196093</v>
+      </c>
+      <c r="B5">
+        <v>-29.922797760999899</v>
+      </c>
+      <c r="C5">
+        <v>350014.04459131049</v>
+      </c>
+      <c r="D5">
+        <v>6688754.5934853461</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>115.445731373</v>
+      </c>
+      <c r="B6">
+        <v>-29.9158760709999</v>
+      </c>
+      <c r="C6">
+        <v>349958.79845159769</v>
+      </c>
+      <c r="D6">
+        <v>6689521.0991102513</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>115.444781776</v>
+      </c>
+      <c r="B7">
+        <v>-29.897913542999898</v>
+      </c>
+      <c r="C7">
+        <v>349840.16920772311</v>
+      </c>
+      <c r="D7">
+        <v>6691510.5949937887</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>115.444467527</v>
+      </c>
+      <c r="B8">
+        <v>-29.893258313999901</v>
+      </c>
+      <c r="C8">
+        <v>349802.84089186718</v>
+      </c>
+      <c r="D8">
+        <v>6692026.1095577255</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>115.443902988</v>
+      </c>
+      <c r="B9">
+        <v>-29.886795741999901</v>
+      </c>
+      <c r="C9">
+        <v>349738.62797378813</v>
+      </c>
+      <c r="D9">
+        <v>6692741.5988855846</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>115.443256772</v>
+      </c>
+      <c r="B10">
+        <v>-29.8811125359999</v>
+      </c>
+      <c r="C10">
+        <v>349667.6909205321</v>
+      </c>
+      <c r="D10">
+        <v>6693370.6060119439</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>115.442575639</v>
+      </c>
+      <c r="B11">
+        <v>-29.876272757999899</v>
+      </c>
+      <c r="C11">
+        <v>349594.64172003686</v>
+      </c>
+      <c r="D11">
+        <v>6693906.0923896097</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>115.44165114400001</v>
+      </c>
+      <c r="B12">
+        <v>-29.870978780999899</v>
+      </c>
+      <c r="C12">
+        <v>349497.39886255271</v>
+      </c>
+      <c r="D12">
+        <v>6694491.5971065024</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>115.44063882099999</v>
+      </c>
+      <c r="B13">
+        <v>-29.866310926999901</v>
+      </c>
+      <c r="C13">
+        <v>349392.6047242973</v>
+      </c>
+      <c r="D13">
+        <v>6695007.5947889313</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>115.43975789300001</v>
+      </c>
+      <c r="B14">
+        <v>-29.862718308999899</v>
+      </c>
+      <c r="C14">
+        <v>349302.11127388396</v>
+      </c>
+      <c r="D14">
+        <v>6695404.5988647295</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>115.43874595699999</v>
+      </c>
+      <c r="B15">
+        <v>-29.858957259999901</v>
+      </c>
+      <c r="C15">
+        <v>349198.70337901684</v>
+      </c>
+      <c r="D15">
+        <v>6695820.0971695855</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>115.437183215</v>
+      </c>
+      <c r="B16">
+        <v>-29.853935444999902</v>
+      </c>
+      <c r="C16">
+        <v>349040.18009686854</v>
+      </c>
+      <c r="D16">
+        <v>6696374.5984358322</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>115.436297963</v>
+      </c>
+      <c r="B17">
+        <v>-29.8515067579999</v>
+      </c>
+      <c r="C17">
+        <v>348951.0011396904</v>
+      </c>
+      <c r="D17">
+        <v>6696642.5997312851</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>115.435318036</v>
+      </c>
+      <c r="B18">
+        <v>-29.849117575999902</v>
+      </c>
+      <c r="C18">
+        <v>348852.73111165967</v>
+      </c>
+      <c r="D18">
+        <v>6696906.0978383264</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>115.43360699199999</v>
+      </c>
+      <c r="B19">
+        <v>-29.845510649999898</v>
+      </c>
+      <c r="C19">
+        <v>348681.98408030928</v>
+      </c>
+      <c r="D19">
+        <v>6697303.5924728923</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>115.431537385</v>
+      </c>
+      <c r="B20">
+        <v>-29.841745832999901</v>
+      </c>
+      <c r="C20">
+        <v>348476.34340665193</v>
+      </c>
+      <c r="D20">
+        <v>6697718.1113115624</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>115.429157096</v>
+      </c>
+      <c r="B21">
+        <v>-29.8378376389999</v>
+      </c>
+      <c r="C21">
+        <v>348240.4526095856</v>
+      </c>
+      <c r="D21">
+        <v>6698148.1071810741</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>115.42668356599999</v>
+      </c>
+      <c r="B22">
+        <v>-29.834031936999899</v>
+      </c>
+      <c r="C22">
+        <v>347995.69012754323</v>
+      </c>
+      <c r="D22">
+        <v>6698566.6166146472</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>115.42079354800001</v>
+      </c>
+      <c r="B23">
+        <v>-29.825403248999901</v>
+      </c>
+      <c r="C23">
+        <v>347413.44482333376</v>
+      </c>
+      <c r="D23">
+        <v>6699515.1139303204</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>115.41854498799999</v>
+      </c>
+      <c r="B24">
+        <v>-29.8219927079999</v>
+      </c>
+      <c r="C24">
+        <v>347190.965810664</v>
+      </c>
+      <c r="D24">
+        <v>6699890.111118298</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>115.41518942</v>
+      </c>
+      <c r="B25">
+        <v>-29.816628733999899</v>
+      </c>
+      <c r="C25">
+        <v>346858.51124945935</v>
+      </c>
+      <c r="D25">
+        <v>6700480.1253548525</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>115.411896185</v>
+      </c>
+      <c r="B26">
+        <v>-29.811121182999901</v>
+      </c>
+      <c r="C26">
+        <v>346531.82817530539</v>
+      </c>
+      <c r="D26">
+        <v>6701086.1258613532</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>115.40927537</v>
+      </c>
+      <c r="B27">
+        <v>-29.806505869999899</v>
+      </c>
+      <c r="C27">
+        <v>346271.46845122473</v>
+      </c>
+      <c r="D27">
+        <v>6701594.1313904785</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>115.407368132</v>
+      </c>
+      <c r="B28">
+        <v>-29.802855687999902</v>
+      </c>
+      <c r="C28">
+        <v>346081.53708889242</v>
+      </c>
+      <c r="D28">
+        <v>6701996.1226181593</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>115.405516636</v>
+      </c>
+      <c r="B29">
+        <v>-29.798822506999901</v>
+      </c>
+      <c r="C29">
+        <v>345896.39372100722</v>
+      </c>
+      <c r="D29">
+        <v>6702440.6319808792</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>115.40416916300001</v>
+      </c>
+      <c r="B30">
+        <v>-29.795427013999898</v>
+      </c>
+      <c r="C30">
+        <v>345760.93621659058</v>
+      </c>
+      <c r="D30">
+        <v>6702815.1404193025</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A31">
+        <v>115.402393281</v>
+      </c>
+      <c r="B31">
+        <v>-29.7903797019999</v>
+      </c>
+      <c r="C31">
+        <v>345581.52046789497</v>
+      </c>
+      <c r="D31">
+        <v>6703372.1390192993</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A32">
+        <v>115.39614165</v>
+      </c>
+      <c r="B32">
+        <v>-29.7717433739999</v>
+      </c>
+      <c r="C32">
+        <v>344948.45764815365</v>
+      </c>
+      <c r="D32">
+        <v>6705429.1488264175</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A33">
+        <v>115.39497130700001</v>
+      </c>
+      <c r="B33">
+        <v>-29.7678807919999</v>
+      </c>
+      <c r="C33">
+        <v>344829.34503770329</v>
+      </c>
+      <c r="D33">
+        <v>6705855.6512027271</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A34">
+        <v>115.39442989299999</v>
+      </c>
+      <c r="B34">
+        <v>-29.7657943419999</v>
+      </c>
+      <c r="C34">
+        <v>344773.77746134496</v>
+      </c>
+      <c r="D34">
+        <v>6706086.1565577202</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A35">
+        <v>115.394053712</v>
+      </c>
+      <c r="B35">
+        <v>-29.764030222999899</v>
+      </c>
+      <c r="C35">
+        <v>344734.68226840068</v>
+      </c>
+      <c r="D35">
+        <v>6706281.1612682072</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A36">
+        <v>115.39370599</v>
+      </c>
+      <c r="B36">
+        <v>-29.761734100999899</v>
+      </c>
+      <c r="C36">
+        <v>344697.5170802502</v>
+      </c>
+      <c r="D36">
+        <v>6706535.1641076989</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A37">
+        <v>115.39345039200001</v>
+      </c>
+      <c r="B37">
+        <v>-29.7588706539999</v>
+      </c>
+      <c r="C37">
+        <v>344668.38359677221</v>
+      </c>
+      <c r="D37">
+        <v>6706852.1653668322</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A38">
+        <v>115.393317592</v>
+      </c>
+      <c r="B38">
+        <v>-29.755683857999902</v>
+      </c>
+      <c r="C38">
+        <v>344650.62505900231</v>
+      </c>
+      <c r="D38">
+        <v>6707205.167364575</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A39">
+        <v>115.39336759299999</v>
+      </c>
+      <c r="B39">
+        <v>-29.753843799999899</v>
+      </c>
+      <c r="C39">
+        <v>344652.62159267964</v>
+      </c>
+      <c r="D39">
+        <v>6707409.1614009198</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A40">
+        <v>115.39353860200001</v>
+      </c>
+      <c r="B40">
+        <v>-29.7528035539999</v>
+      </c>
+      <c r="C40">
+        <v>344667.5543278947</v>
+      </c>
+      <c r="D40">
+        <v>6707524.6781176822</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A41">
+        <v>115.39380685499999</v>
+      </c>
+      <c r="B41">
+        <v>-29.752039930999899</v>
+      </c>
+      <c r="C41">
+        <v>344692.3181543044</v>
+      </c>
+      <c r="D41">
+        <v>6707609.6685717218</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A42">
+        <v>115.39569038400001</v>
+      </c>
+      <c r="B42">
+        <v>-29.7484309489999</v>
+      </c>
+      <c r="C42">
+        <v>344868.90782163257</v>
+      </c>
+      <c r="D42">
+        <v>6708012.1711618342</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A43">
+        <v>115.39841556899999</v>
+      </c>
+      <c r="B43">
+        <v>-29.753963601999899</v>
+      </c>
+      <c r="C43">
+        <v>345140.96628398867</v>
+      </c>
+      <c r="D43">
+        <v>6707402.6685904097</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A44">
+        <v>115.401367182</v>
+      </c>
+      <c r="B44">
+        <v>-29.7604373379999</v>
+      </c>
+      <c r="C44">
+        <v>345436.33712689026</v>
+      </c>
+      <c r="D44">
+        <v>6706689.1669161683</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A45">
+        <v>115.40384761599999</v>
+      </c>
+      <c r="B45">
+        <v>-29.7537225139999</v>
+      </c>
+      <c r="C45">
+        <v>345665.8972145358</v>
+      </c>
+      <c r="D45">
+        <v>6707436.6641048854</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A46">
+        <v>115.40473681100001</v>
+      </c>
+      <c r="B46">
+        <v>-29.7509585829999</v>
+      </c>
+      <c r="C46">
+        <v>345747.65257992124</v>
+      </c>
+      <c r="D46">
+        <v>6707744.1680321768</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A47">
+        <v>115.405594331</v>
+      </c>
+      <c r="B47">
+        <v>-29.747698018999898</v>
+      </c>
+      <c r="C47">
+        <v>345825.58957002906</v>
+      </c>
+      <c r="D47">
+        <v>6708106.6684881281</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A48">
+        <v>115.406321906</v>
+      </c>
+      <c r="B48">
+        <v>-29.7445621389999</v>
+      </c>
+      <c r="C48">
+        <v>345891.15578620124</v>
+      </c>
+      <c r="D48">
+        <v>6708455.1763473861</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A49">
+        <v>115.40687667100001</v>
+      </c>
+      <c r="B49">
+        <v>-29.741703892999901</v>
+      </c>
+      <c r="C49">
+        <v>345940.43790150841</v>
+      </c>
+      <c r="D49">
+        <v>6708772.6839208361</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A50">
+        <v>115.407151054</v>
+      </c>
+      <c r="B50">
+        <v>-29.739749195999899</v>
+      </c>
+      <c r="C50">
+        <v>345963.98665474227</v>
+      </c>
+      <c r="D50">
+        <v>6708989.6806041524</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A51">
+        <v>115.4073642</v>
+      </c>
+      <c r="B51">
+        <v>-29.737446259999899</v>
+      </c>
+      <c r="C51">
+        <v>345981.08154434757</v>
+      </c>
+      <c r="D51">
+        <v>6709245.1892475821</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A52">
+        <v>115.407606839</v>
+      </c>
+      <c r="B52">
+        <v>-29.7327165079999</v>
+      </c>
+      <c r="C52">
+        <v>345997.32193767821</v>
+      </c>
+      <c r="D52">
+        <v>6709769.6902566459</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A53">
+        <v>115.408204873</v>
+      </c>
+      <c r="B53">
+        <v>-29.7107249019999</v>
+      </c>
+      <c r="C53">
+        <v>346021.58716536767</v>
+      </c>
+      <c r="D53">
+        <v>6712207.7145963777</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A54">
+        <v>115.408586183</v>
+      </c>
+      <c r="B54">
+        <v>-29.702112274999902</v>
+      </c>
+      <c r="C54">
+        <v>346045.33577085158</v>
+      </c>
+      <c r="D54">
+        <v>6713162.7177105742</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A55">
+        <v>115.40883138300001</v>
+      </c>
+      <c r="B55">
+        <v>-29.698487642999901</v>
+      </c>
+      <c r="C55">
+        <v>346063.53108937381</v>
+      </c>
+      <c r="D55">
+        <v>6713564.744040681</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A56">
+        <v>115.40927883800001</v>
+      </c>
+      <c r="B56">
+        <v>-29.693611568999899</v>
+      </c>
+      <c r="C56">
+        <v>346099.39109140029</v>
+      </c>
+      <c r="D56">
+        <v>6714105.7302161008</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A57">
+        <v>115.410483403</v>
+      </c>
+      <c r="B57">
+        <v>-29.683880810999899</v>
+      </c>
+      <c r="C57">
+        <v>346201.12519219232</v>
+      </c>
+      <c r="D57">
+        <v>6715185.7418865878</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A58">
+        <v>115.410844858</v>
+      </c>
+      <c r="B58">
+        <v>-29.680420117999901</v>
+      </c>
+      <c r="C58">
+        <v>346230.83458415989</v>
+      </c>
+      <c r="D58">
+        <v>6715569.7525736922</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A59">
+        <v>115.41123693999999</v>
+      </c>
+      <c r="B59">
+        <v>-29.673179125999901</v>
+      </c>
+      <c r="C59">
+        <v>346257.75803754723</v>
+      </c>
+      <c r="D59">
+        <v>6716372.7534396239</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A60">
+        <v>115.41163113499999</v>
+      </c>
+      <c r="B60">
+        <v>-29.668388070999899</v>
+      </c>
+      <c r="C60">
+        <v>346288.62040975341</v>
+      </c>
+      <c r="D60">
+        <v>6716904.2432403928</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A61">
+        <v>115.412331722</v>
+      </c>
+      <c r="B61">
+        <v>-29.653891520999899</v>
+      </c>
+      <c r="C61">
+        <v>346334.39094691665</v>
+      </c>
+      <c r="D61">
+        <v>6718511.7434191797</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A62">
+        <v>115.413000626</v>
+      </c>
+      <c r="B62">
+        <v>-29.645408521999901</v>
+      </c>
+      <c r="C62">
+        <v>346386.25555911945</v>
+      </c>
+      <c r="D62">
+        <v>6719452.7517524641</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A63">
+        <v>115.41375521400001</v>
+      </c>
+      <c r="B63">
+        <v>-29.638943329999901</v>
+      </c>
+      <c r="C63">
+        <v>346449.49232106155</v>
+      </c>
+      <c r="D63">
+        <v>6720170.2506856238</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A64">
+        <v>115.414166338</v>
+      </c>
+      <c r="B64">
+        <v>-29.636408201999899</v>
+      </c>
+      <c r="C64">
+        <v>346485.44844035164</v>
+      </c>
+      <c r="D64">
+        <v>6720451.7483870191</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A65">
+        <v>115.414615587</v>
+      </c>
+      <c r="B65">
+        <v>-29.6341487659999</v>
+      </c>
+      <c r="C65">
+        <v>346525.51619945152</v>
+      </c>
+      <c r="D65">
+        <v>6720702.7430717181</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A66">
+        <v>115.415614588</v>
+      </c>
+      <c r="B66">
+        <v>-29.630262512999899</v>
+      </c>
+      <c r="C66">
+        <v>346616.34797813557</v>
+      </c>
+      <c r="D66">
+        <v>6721134.7554212119</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A67">
+        <v>115.41733539499999</v>
+      </c>
+      <c r="B67">
+        <v>-29.625126325999901</v>
+      </c>
+      <c r="C67">
+        <v>346775.18544546037</v>
+      </c>
+      <c r="D67">
+        <v>6721706.2434763554</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A68">
+        <v>115.417746147</v>
+      </c>
+      <c r="B68">
+        <v>-29.623231767999901</v>
+      </c>
+      <c r="C68">
+        <v>346812.09054440231</v>
+      </c>
+      <c r="D68">
+        <v>6721916.7482728399</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A69">
+        <v>115.418153718</v>
+      </c>
+      <c r="B69">
+        <v>-29.6200738819999</v>
+      </c>
+      <c r="C69">
+        <v>346846.77831066458</v>
+      </c>
+      <c r="D69">
+        <v>6722267.2550489744</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A70">
+        <v>115.419109867</v>
+      </c>
+      <c r="B70">
+        <v>-29.610944624999899</v>
+      </c>
+      <c r="C70">
+        <v>346925.56531583972</v>
+      </c>
+      <c r="D70">
+        <v>6723280.2535439245</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A71">
+        <v>115.419587249</v>
+      </c>
+      <c r="B71">
+        <v>-29.6070568049999</v>
+      </c>
+      <c r="C71">
+        <v>346965.92186802003</v>
+      </c>
+      <c r="D71">
+        <v>6723711.7448178902</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A72">
+        <v>115.420136633</v>
+      </c>
+      <c r="B72">
+        <v>-29.603679545999899</v>
+      </c>
+      <c r="C72">
+        <v>347014.0268440072</v>
+      </c>
+      <c r="D72">
+        <v>6724086.7485863306</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A73">
+        <v>115.420874633</v>
+      </c>
+      <c r="B73">
+        <v>-29.600367725999899</v>
+      </c>
+      <c r="C73">
+        <v>347080.50226009131</v>
+      </c>
+      <c r="D73">
+        <v>6724454.7484378032</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A74">
+        <v>115.421914333</v>
+      </c>
+      <c r="B74">
+        <v>-29.596576667999901</v>
+      </c>
+      <c r="C74">
+        <v>347175.48100956762</v>
+      </c>
+      <c r="D74">
+        <v>6724876.2557725143</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A75">
+        <v>115.424196706</v>
+      </c>
+      <c r="B75">
+        <v>-29.5888977769999</v>
+      </c>
+      <c r="C75">
+        <v>347384.97764928488</v>
+      </c>
+      <c r="D75">
+        <v>6725730.2583726691</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A76">
+        <v>115.42557621900001</v>
+      </c>
+      <c r="B76">
+        <v>-29.584023461999902</v>
+      </c>
+      <c r="C76">
+        <v>347511.26878070942</v>
+      </c>
+      <c r="D76">
+        <v>6726272.2577015385</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A77">
+        <v>115.42677178700001</v>
+      </c>
+      <c r="B77">
+        <v>-29.5793500159999</v>
+      </c>
+      <c r="C77">
+        <v>347620.05671106605</v>
+      </c>
+      <c r="D77">
+        <v>6726791.7523119096</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A78">
+        <v>115.42851387100001</v>
+      </c>
+      <c r="B78">
+        <v>-29.5721066669999</v>
+      </c>
+      <c r="C78">
+        <v>347777.94387976115</v>
+      </c>
+      <c r="D78">
+        <v>6727596.7651166935</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A79">
+        <v>115.429945631</v>
+      </c>
+      <c r="B79">
+        <v>-29.566754649999901</v>
+      </c>
+      <c r="C79">
+        <v>347908.6267117348</v>
+      </c>
+      <c r="D79">
+        <v>6728191.7655096445</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A80">
+        <v>115.43101082299999</v>
+      </c>
+      <c r="B80">
+        <v>-29.5632164619999</v>
+      </c>
+      <c r="C80">
+        <v>348006.52597550198</v>
+      </c>
+      <c r="D80">
+        <v>6728585.2708486766</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A81">
+        <v>115.432205689</v>
+      </c>
+      <c r="B81">
+        <v>-29.5596167019999</v>
+      </c>
+      <c r="C81">
+        <v>348116.9048908581</v>
+      </c>
+      <c r="D81">
+        <v>6728985.7680350207</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A82">
+        <v>115.433080128</v>
+      </c>
+      <c r="B82">
+        <v>-29.557366640999899</v>
+      </c>
+      <c r="C82">
+        <v>348198.26384712814</v>
+      </c>
+      <c r="D82">
+        <v>6729236.268233262</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A83">
+        <v>115.43387644000001</v>
+      </c>
+      <c r="B83">
+        <v>-29.555747267999902</v>
+      </c>
+      <c r="C83">
+        <v>348272.99937977019</v>
+      </c>
+      <c r="D83">
+        <v>6729416.7713790592</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A84">
+        <v>115.435677117</v>
+      </c>
+      <c r="B84">
+        <v>-29.552750202999899</v>
+      </c>
+      <c r="C84">
+        <v>348442.99845051504</v>
+      </c>
+      <c r="D84">
+        <v>6729751.2637446821</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A85">
+        <v>115.437575064</v>
+      </c>
+      <c r="B85">
+        <v>-29.550096970999899</v>
+      </c>
+      <c r="C85">
+        <v>348622.94609043794</v>
+      </c>
+      <c r="D85">
+        <v>6730047.7755479012</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A86">
+        <v>115.43856906400001</v>
+      </c>
+      <c r="B86">
+        <v>-29.548895002999899</v>
+      </c>
+      <c r="C86">
+        <v>348717.47235830239</v>
+      </c>
+      <c r="D86">
+        <v>6730182.2751127277</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A87">
+        <v>115.439554688</v>
+      </c>
+      <c r="B87">
+        <v>-29.547832823999901</v>
+      </c>
+      <c r="C87">
+        <v>348811.39742986072</v>
+      </c>
+      <c r="D87">
+        <v>6730301.2711953958</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A88">
+        <v>115.44117112000001</v>
+      </c>
+      <c r="B88">
+        <v>-29.5464215689999</v>
+      </c>
+      <c r="C88">
+        <v>348965.93161719933</v>
+      </c>
+      <c r="D88">
+        <v>6730459.772067342</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A89">
+        <v>115.441828117</v>
+      </c>
+      <c r="B89">
+        <v>-29.545964628999901</v>
+      </c>
+      <c r="C89">
+        <v>349028.91654576914</v>
+      </c>
+      <c r="D89">
+        <v>6730511.2651089178</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A90">
+        <v>115.44286204799999</v>
+      </c>
+      <c r="B90">
+        <v>-29.5453675609999</v>
+      </c>
+      <c r="C90">
+        <v>349128.21978631616</v>
+      </c>
+      <c r="D90">
+        <v>6730578.7766687637</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A91">
+        <v>115.444445671</v>
+      </c>
+      <c r="B91">
+        <v>-29.544673306999901</v>
+      </c>
+      <c r="C91">
+        <v>349280.6469543596</v>
+      </c>
+      <c r="D91">
+        <v>6730657.7710210793</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A92">
+        <v>115.44659235899999</v>
+      </c>
+      <c r="B92">
+        <v>-29.543967431999899</v>
+      </c>
+      <c r="C92">
+        <v>349487.62222937343</v>
+      </c>
+      <c r="D92">
+        <v>6730738.7808233136</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A93">
+        <v>115.451888318</v>
+      </c>
+      <c r="B93">
+        <v>-29.5424139879999</v>
+      </c>
+      <c r="C93">
+        <v>349998.52752149745</v>
+      </c>
+      <c r="D93">
+        <v>6730917.7864369117</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A94">
+        <v>115.45100487099999</v>
+      </c>
+      <c r="B94">
+        <v>-29.539561298999899</v>
+      </c>
+      <c r="C94">
+        <v>349908.70171415759</v>
+      </c>
+      <c r="D94">
+        <v>6731232.7841716278</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A95">
+        <v>115.453782999</v>
+      </c>
+      <c r="B95">
+        <v>-29.535745164999899</v>
+      </c>
+      <c r="C95">
+        <v>350172.29695395409</v>
+      </c>
+      <c r="D95">
+        <v>6731659.2789890356</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A96">
+        <v>115.454373746</v>
+      </c>
+      <c r="B96">
+        <v>-29.534804602999898</v>
+      </c>
+      <c r="C96">
+        <v>350228.16078479879</v>
+      </c>
+      <c r="D96">
+        <v>6731764.2748539783</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A97">
+        <v>115.45516142699999</v>
+      </c>
+      <c r="B97">
+        <v>-29.5332661049999</v>
+      </c>
+      <c r="C97">
+        <v>350302.23035519291</v>
+      </c>
+      <c r="D97">
+        <v>6731935.7880733889</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A98">
+        <v>115.45584723899999</v>
+      </c>
+      <c r="B98">
+        <v>-29.531667917999901</v>
+      </c>
+      <c r="C98">
+        <v>350366.3417546266</v>
+      </c>
+      <c r="D98">
+        <v>6732113.7842958691</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A99">
+        <v>115.457257676</v>
+      </c>
+      <c r="B99">
+        <v>-29.527921418999899</v>
+      </c>
+      <c r="C99">
+        <v>350497.52360750636</v>
+      </c>
+      <c r="D99">
+        <v>6732530.7906018011</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A100">
+        <v>115.460333545</v>
+      </c>
+      <c r="B100">
+        <v>-29.518942486999901</v>
+      </c>
+      <c r="C100">
+        <v>350782.45414930908</v>
+      </c>
+      <c r="D100">
+        <v>6733529.7964607906</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A101">
+        <v>115.463226085</v>
+      </c>
+      <c r="B101">
+        <v>-29.510890793999899</v>
+      </c>
+      <c r="C101">
+        <v>351051.02758255496</v>
+      </c>
+      <c r="D101">
+        <v>6734425.799710813</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A102">
+        <v>115.464910567</v>
+      </c>
+      <c r="B102">
+        <v>-29.505748736999902</v>
+      </c>
+      <c r="C102">
+        <v>351206.79132767639</v>
+      </c>
+      <c r="D102">
+        <v>6734997.8016453134</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A103">
+        <v>115.46654098</v>
+      </c>
+      <c r="B103">
+        <v>-29.500001418999901</v>
+      </c>
+      <c r="C103">
+        <v>351356.44679101353</v>
+      </c>
+      <c r="D103">
+        <v>6735636.8064557258</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A104">
+        <v>115.468289071</v>
+      </c>
+      <c r="B104">
+        <v>-29.492942372999899</v>
+      </c>
+      <c r="C104">
+        <v>351515.61684755632</v>
+      </c>
+      <c r="D104">
+        <v>6736421.3241544245</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A105">
+        <v>115.469519174</v>
+      </c>
+      <c r="B105">
+        <v>-29.487072994999899</v>
+      </c>
+      <c r="C105">
+        <v>351626.3229185837</v>
+      </c>
+      <c r="D105">
+        <v>6737073.3384575285</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A106">
+        <v>115.469986476</v>
+      </c>
+      <c r="B106">
+        <v>-29.484312634999899</v>
+      </c>
+      <c r="C106">
+        <v>351667.60978873953</v>
+      </c>
+      <c r="D106">
+        <v>6737379.8373323195</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A107">
+        <v>115.470257898</v>
+      </c>
+      <c r="B107">
+        <v>-29.4821410099999</v>
+      </c>
+      <c r="C107">
+        <v>351690.76384108409</v>
+      </c>
+      <c r="D107">
+        <v>6737620.8426569272</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A108">
+        <v>115.47035720700001</v>
+      </c>
+      <c r="B108">
+        <v>-29.480445825999901</v>
+      </c>
+      <c r="C108">
+        <v>351697.92423544056</v>
+      </c>
+      <c r="D108">
+        <v>6737808.8293672688</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A109">
+        <v>115.47027263299999</v>
+      </c>
+      <c r="B109">
+        <v>-29.478671726999899</v>
+      </c>
+      <c r="C109">
+        <v>351687.13981253211</v>
+      </c>
+      <c r="D109">
+        <v>6738005.3270612927</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A110">
+        <v>115.47005407</v>
+      </c>
+      <c r="B110">
+        <v>-29.477532151999899</v>
+      </c>
+      <c r="C110">
+        <v>351664.28685523046</v>
+      </c>
+      <c r="D110">
+        <v>6738131.3360936567</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A111">
+        <v>115.46966819799999</v>
+      </c>
+      <c r="B111">
+        <v>-29.476458463999901</v>
+      </c>
+      <c r="C111">
+        <v>351625.30585811543</v>
+      </c>
+      <c r="D111">
+        <v>6738249.830229356</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A112">
+        <v>115.468836939</v>
+      </c>
+      <c r="B112">
+        <v>-29.4750186559999</v>
+      </c>
+      <c r="C112">
+        <v>351542.60178327037</v>
+      </c>
+      <c r="D112">
+        <v>6738408.3296539448</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A113">
+        <v>115.46770943999999</v>
+      </c>
+      <c r="B113">
+        <v>-29.4736114859999</v>
+      </c>
+      <c r="C113">
+        <v>351431.21652082534</v>
+      </c>
+      <c r="D113">
+        <v>6738562.8335455721</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A114">
+        <v>115.466475679</v>
+      </c>
+      <c r="B114">
+        <v>-29.472419592999898</v>
+      </c>
+      <c r="C114">
+        <v>351309.8380919834</v>
+      </c>
+      <c r="D114">
+        <v>6738693.3437382802</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A115">
+        <v>115.465167436</v>
+      </c>
+      <c r="B115">
+        <v>-29.4715112159999</v>
+      </c>
+      <c r="C115">
+        <v>351181.64833395998</v>
+      </c>
+      <c r="D115">
+        <v>6738792.3382915761</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A116">
+        <v>115.463528001</v>
+      </c>
+      <c r="B116">
+        <v>-29.470734283999899</v>
+      </c>
+      <c r="C116">
+        <v>351021.53165686422</v>
+      </c>
+      <c r="D116">
+        <v>6738876.3409648258</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A117">
+        <v>115.46189393</v>
+      </c>
+      <c r="B117">
+        <v>-29.470133403999899</v>
+      </c>
+      <c r="C117">
+        <v>350862.19041719695</v>
+      </c>
+      <c r="D117">
+        <v>6738940.8382503251</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A118">
+        <v>115.45979262100001</v>
+      </c>
+      <c r="B118">
+        <v>-29.469491043999898</v>
+      </c>
+      <c r="C118">
+        <v>350657.47618786746</v>
+      </c>
+      <c r="D118">
+        <v>6739009.3309014561</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A119">
+        <v>115.45713618400001</v>
+      </c>
+      <c r="B119">
+        <v>-29.468815026999899</v>
+      </c>
+      <c r="C119">
+        <v>350398.87611023244</v>
+      </c>
+      <c r="D119">
+        <v>6739080.8366149152</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A120">
+        <v>115.446816449</v>
+      </c>
+      <c r="B120">
+        <v>-29.4666015889999</v>
+      </c>
+      <c r="C120">
+        <v>349394.84195469244</v>
+      </c>
+      <c r="D120">
+        <v>6739312.8256406877</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A121">
+        <v>115.438007978</v>
+      </c>
+      <c r="B121">
+        <v>-29.464531206999901</v>
+      </c>
+      <c r="C121">
+        <v>348537.53721464006</v>
+      </c>
+      <c r="D121">
+        <v>6739530.8403183501</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A122">
+        <v>115.42879494100001</v>
+      </c>
+      <c r="B122">
+        <v>-29.4628752449999</v>
+      </c>
+      <c r="C122">
+        <v>347641.57999137964</v>
+      </c>
+      <c r="D122">
+        <v>6739702.3356429208</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A123">
+        <v>115.42816168500001</v>
+      </c>
+      <c r="B123">
+        <v>-29.460972862999899</v>
+      </c>
+      <c r="C123">
+        <v>347577.32029079297</v>
+      </c>
+      <c r="D123">
+        <v>6739912.3303399822</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A124">
+        <v>115.427624929</v>
+      </c>
+      <c r="B124">
+        <v>-29.4590354209999</v>
+      </c>
+      <c r="C124">
+        <v>347522.36509648582</v>
+      </c>
+      <c r="D124">
+        <v>6740126.3364401553</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A125">
+        <v>115.427302364</v>
+      </c>
+      <c r="B125">
+        <v>-29.4581697929999</v>
+      </c>
+      <c r="C125">
+        <v>347489.78567953233</v>
+      </c>
+      <c r="D125">
+        <v>6740221.843599109</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A126">
+        <v>115.426867796</v>
+      </c>
+      <c r="B126">
+        <v>-29.4571585539999</v>
+      </c>
+      <c r="C126">
+        <v>347446.12497409596</v>
+      </c>
+      <c r="D126">
+        <v>6740333.3406871893</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A127">
+        <v>115.42443851</v>
+      </c>
+      <c r="B127">
+        <v>-29.450479374999901</v>
+      </c>
+      <c r="C127">
+        <v>347200.50383655494</v>
+      </c>
+      <c r="D127">
+        <v>6741070.3477616115</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A128">
+        <v>115.42050039</v>
+      </c>
+      <c r="B128">
+        <v>-29.4406916289999</v>
+      </c>
+      <c r="C128">
+        <v>346803.82731720299</v>
+      </c>
+      <c r="D128">
+        <v>6742149.8607412744</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A129">
+        <v>115.416572776</v>
+      </c>
+      <c r="B129">
+        <v>-29.431454160999898</v>
+      </c>
+      <c r="C129">
+        <v>346408.92906327848</v>
+      </c>
+      <c r="D129">
+        <v>6743168.3931622375</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A130">
+        <v>115.414711219</v>
+      </c>
+      <c r="B130">
+        <v>-29.427294656999901</v>
+      </c>
+      <c r="C130">
+        <v>346222.06733357639</v>
+      </c>
+      <c r="D130">
+        <v>6743626.8975614402</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A131">
+        <v>115.412984634</v>
+      </c>
+      <c r="B131">
+        <v>-29.423628595999901</v>
+      </c>
+      <c r="C131">
+        <v>346049.03086411091</v>
+      </c>
+      <c r="D131">
+        <v>6744030.8938304717</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A132">
+        <v>115.410511055</v>
+      </c>
+      <c r="B132">
+        <v>-29.4187985249999</v>
+      </c>
+      <c r="C132">
+        <v>345801.7490028296</v>
+      </c>
+      <c r="D132">
+        <v>6744562.8964086305</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A133">
+        <v>115.40791541199999</v>
+      </c>
+      <c r="B133">
+        <v>-29.4142287079999</v>
+      </c>
+      <c r="C133">
+        <v>345542.99532580451</v>
+      </c>
+      <c r="D133">
+        <v>6745065.8910343386</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A134">
+        <v>115.405027451</v>
+      </c>
+      <c r="B134">
+        <v>-29.4095198979999</v>
+      </c>
+      <c r="C134">
+        <v>345255.64479688311</v>
+      </c>
+      <c r="D134">
+        <v>6745583.8958852571</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A135">
+        <v>115.400985742</v>
+      </c>
+      <c r="B135">
+        <v>-29.4033761889999</v>
+      </c>
+      <c r="C135">
+        <v>344854.1327827333</v>
+      </c>
+      <c r="D135">
+        <v>6746259.3767302958</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A136">
+        <v>115.398145668</v>
+      </c>
+      <c r="B136">
+        <v>-29.3993851339999</v>
+      </c>
+      <c r="C136">
+        <v>344572.46240551642</v>
+      </c>
+      <c r="D136">
+        <v>6746697.8876605481</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A137">
+        <v>115.39560296099999</v>
+      </c>
+      <c r="B137">
+        <v>-29.396110564999901</v>
+      </c>
+      <c r="C137">
+        <v>344320.72117229691</v>
+      </c>
+      <c r="D137">
+        <v>6747057.3876015861</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A138">
+        <v>115.393252508</v>
+      </c>
+      <c r="B138">
+        <v>-29.393361627999901</v>
+      </c>
+      <c r="C138">
+        <v>344088.42452295625</v>
+      </c>
+      <c r="D138">
+        <v>6747358.8884496987</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A139">
+        <v>115.390056814</v>
+      </c>
+      <c r="B139">
+        <v>-29.389961820999901</v>
+      </c>
+      <c r="C139">
+        <v>343773.08901266556</v>
+      </c>
+      <c r="D139">
+        <v>6747731.3836352378</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A140">
+        <v>115.384486486</v>
+      </c>
+      <c r="B140">
+        <v>-29.384565944999899</v>
+      </c>
+      <c r="C140">
+        <v>343224.20069910015</v>
+      </c>
+      <c r="D140">
+        <v>6748321.8895128071</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A141">
+        <v>115.368062169</v>
+      </c>
+      <c r="B141">
+        <v>-29.3694586989999</v>
+      </c>
+      <c r="C141">
+        <v>341606.69738010515</v>
+      </c>
+      <c r="D141">
+        <v>6749973.9196505276</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A142">
+        <v>115.362405471</v>
+      </c>
+      <c r="B142">
+        <v>-29.364137633999899</v>
+      </c>
+      <c r="C142">
+        <v>341049.32170999702</v>
+      </c>
+      <c r="D142">
+        <v>6750555.9203832317</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A143">
+        <v>115.36104033700001</v>
+      </c>
+      <c r="B143">
+        <v>-29.3575110539999</v>
+      </c>
+      <c r="C143">
+        <v>340906.49552729254</v>
+      </c>
+      <c r="D143">
+        <v>6751288.4267490366</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A144">
+        <v>115.360624526</v>
+      </c>
+      <c r="B144">
+        <v>-29.355764383999901</v>
+      </c>
+      <c r="C144">
+        <v>340863.41112308297</v>
+      </c>
+      <c r="D144">
+        <v>6751481.4282238511</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A145">
+        <v>115.35791589599999</v>
+      </c>
+      <c r="B145">
+        <v>-29.345981110999901</v>
+      </c>
+      <c r="C145">
+        <v>340585.2080769348</v>
+      </c>
+      <c r="D145">
+        <v>6752561.9281985108</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A146">
+        <v>115.356258442</v>
+      </c>
+      <c r="B146">
+        <v>-29.339567339999899</v>
+      </c>
+      <c r="C146">
+        <v>340414.28284290514</v>
+      </c>
+      <c r="D146">
+        <v>6753270.4464460583</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A147">
+        <v>115.354573618</v>
+      </c>
+      <c r="B147">
+        <v>-29.3324767229999</v>
+      </c>
+      <c r="C147">
+        <v>340239.62599458918</v>
+      </c>
+      <c r="D147">
+        <v>6754053.9336642604</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A148">
+        <v>115.353084662</v>
+      </c>
+      <c r="B148">
+        <v>-29.325699610999902</v>
+      </c>
+      <c r="C148">
+        <v>340084.45969390031</v>
+      </c>
+      <c r="D148">
+        <v>6754802.9434492532</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A149">
+        <v>115.352246533</v>
+      </c>
+      <c r="B149">
+        <v>-29.3212586749999</v>
+      </c>
+      <c r="C149">
+        <v>339996.1320910987</v>
+      </c>
+      <c r="D149">
+        <v>6755293.9450502582</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A150">
+        <v>115.351092386</v>
+      </c>
+      <c r="B150">
+        <v>-29.313470627999902</v>
+      </c>
+      <c r="C150">
+        <v>339871.8778657575</v>
+      </c>
+      <c r="D150">
+        <v>6756155.4426200036</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A151">
+        <v>115.353151579</v>
+      </c>
+      <c r="B151">
+        <v>-29.314474999999899</v>
+      </c>
+      <c r="C151">
+        <v>340073.44513964665</v>
+      </c>
+      <c r="D151">
+        <v>6756046.9544658773</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A152">
+        <v>115.34999541099999</v>
+      </c>
+      <c r="B152">
+        <v>-29.3001201719999</v>
+      </c>
+      <c r="C152">
+        <v>339744.47211196006</v>
+      </c>
+      <c r="D152">
+        <v>6757633.4462269265</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A153">
+        <v>115.347715127</v>
+      </c>
+      <c r="B153">
+        <v>-29.2893402579999</v>
+      </c>
+      <c r="C153">
+        <v>339506.10742351646</v>
+      </c>
+      <c r="D153">
+        <v>6758824.9569011442</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A154">
+        <v>115.346970666</v>
+      </c>
+      <c r="B154">
+        <v>-29.286186266999898</v>
+      </c>
+      <c r="C154">
+        <v>339428.84952992981</v>
+      </c>
+      <c r="D154">
+        <v>6759173.4626249038</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A155">
+        <v>115.34652640900001</v>
+      </c>
+      <c r="B155">
+        <v>-29.284606268999902</v>
+      </c>
+      <c r="C155">
+        <v>339383.21679083107</v>
+      </c>
+      <c r="D155">
+        <v>6759347.9492428079</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A156">
+        <v>115.34584203</v>
+      </c>
+      <c r="B156">
+        <v>-29.2826983369999</v>
+      </c>
+      <c r="C156">
+        <v>339313.74052867468</v>
+      </c>
+      <c r="D156">
+        <v>6759558.4479644401</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A157">
+        <v>115.34501833500001</v>
+      </c>
+      <c r="B157">
+        <v>-29.280951030999901</v>
+      </c>
+      <c r="C157">
+        <v>339230.97800509224</v>
+      </c>
+      <c r="D157">
+        <v>6759750.9544209754</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A158">
+        <v>115.343621204</v>
+      </c>
+      <c r="B158">
+        <v>-29.278483733999899</v>
+      </c>
+      <c r="C158">
+        <v>339091.37037253997</v>
+      </c>
+      <c r="D158">
+        <v>6760022.462223826</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A159">
+        <v>115.342414823</v>
+      </c>
+      <c r="B159">
+        <v>-29.276618974999899</v>
+      </c>
+      <c r="C159">
+        <v>338971.23494724167</v>
+      </c>
+      <c r="D159">
+        <v>6760227.4573217705</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A160">
+        <v>115.34113606699999</v>
+      </c>
+      <c r="B160">
+        <v>-29.274866036999899</v>
+      </c>
+      <c r="C160">
+        <v>338844.2387414379</v>
+      </c>
+      <c r="D160">
+        <v>6760419.959658904</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A161">
+        <v>115.339295741</v>
+      </c>
+      <c r="B161">
+        <v>-29.272677590999901</v>
+      </c>
+      <c r="C161">
+        <v>338661.98966558493</v>
+      </c>
+      <c r="D161">
+        <v>6760659.9504815284</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A162">
+        <v>115.337188666</v>
+      </c>
+      <c r="B162">
+        <v>-29.2704811649999</v>
+      </c>
+      <c r="C162">
+        <v>338453.80141612038</v>
+      </c>
+      <c r="D162">
+        <v>6760900.4551473819</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A163">
+        <v>115.333430268</v>
+      </c>
+      <c r="B163">
+        <v>-29.266802286999901</v>
+      </c>
+      <c r="C163">
+        <v>338082.81033300958</v>
+      </c>
+      <c r="D163">
+        <v>6761302.9610730316</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A164">
+        <v>115.33206113999999</v>
+      </c>
+      <c r="B164">
+        <v>-29.265314410999899</v>
+      </c>
+      <c r="C164">
+        <v>337947.42438738747</v>
+      </c>
+      <c r="D164">
+        <v>6761465.9551366325</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A165">
+        <v>115.331636006</v>
+      </c>
+      <c r="B165">
+        <v>-29.264731461999901</v>
+      </c>
+      <c r="C165">
+        <v>337905.19348831609</v>
+      </c>
+      <c r="D165">
+        <v>6761529.969704574</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A166">
+        <v>115.331199699</v>
+      </c>
+      <c r="B166">
+        <v>-29.263918427999901</v>
+      </c>
+      <c r="C166">
+        <v>337861.51327657176</v>
+      </c>
+      <c r="D166">
+        <v>6761619.466807615</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A167">
+        <v>115.330876014</v>
+      </c>
+      <c r="B167">
+        <v>-29.2630256069999</v>
+      </c>
+      <c r="C167">
+        <v>337828.65039622015</v>
+      </c>
+      <c r="D167">
+        <v>6761717.9616927663</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A168">
+        <v>115.330523261</v>
+      </c>
+      <c r="B168">
+        <v>-29.261676732999899</v>
+      </c>
+      <c r="C168">
+        <v>337792.24229561706</v>
+      </c>
+      <c r="D168">
+        <v>6761866.9562764317</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A169">
+        <v>115.330304328</v>
+      </c>
+      <c r="B169">
+        <v>-29.260302287999899</v>
+      </c>
+      <c r="C169">
+        <v>337768.7971757577</v>
+      </c>
+      <c r="D169">
+        <v>6762018.9698373973</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A170">
+        <v>115.33004120699999</v>
+      </c>
+      <c r="B170">
+        <v>-29.257537792999901</v>
+      </c>
+      <c r="C170">
+        <v>337738.86244432168</v>
+      </c>
+      <c r="D170">
+        <v>6762324.9681421742</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A171">
+        <v>115.33334958099999</v>
+      </c>
+      <c r="B171">
+        <v>-29.259821416999898</v>
+      </c>
+      <c r="C171">
+        <v>338063.96652609354</v>
+      </c>
+      <c r="D171">
+        <v>6762076.4726371309</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A172">
+        <v>115.334507348</v>
+      </c>
+      <c r="B172">
+        <v>-29.2572551549999</v>
+      </c>
+      <c r="C172">
+        <v>338172.43322356563</v>
+      </c>
+      <c r="D172">
+        <v>6762362.4661474535</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A173">
+        <v>115.334843275</v>
+      </c>
+      <c r="B173">
+        <v>-29.255806542999899</v>
+      </c>
+      <c r="C173">
+        <v>338202.79759464721</v>
+      </c>
+      <c r="D173">
+        <v>6762523.4656164041</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A174">
+        <v>115.334954143</v>
+      </c>
+      <c r="B174">
+        <v>-29.2546484299999</v>
+      </c>
+      <c r="C174">
+        <v>338211.74860326346</v>
+      </c>
+      <c r="D174">
+        <v>6762651.9610780086</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A175">
+        <v>115.33496096</v>
+      </c>
+      <c r="B175">
+        <v>-29.2531912329999</v>
+      </c>
+      <c r="C175">
+        <v>338210.11711889808</v>
+      </c>
+      <c r="D175">
+        <v>6762813.4574253112</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A176">
+        <v>115.334872773</v>
+      </c>
+      <c r="B176">
+        <v>-29.252044112999901</v>
+      </c>
+      <c r="C176">
+        <v>338199.74096193037</v>
+      </c>
+      <c r="D176">
+        <v>6762940.4597870708</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A177">
+        <v>115.33468302999999</v>
+      </c>
+      <c r="B177">
+        <v>-29.250760363999898</v>
+      </c>
+      <c r="C177">
+        <v>338179.27981673682</v>
+      </c>
+      <c r="D177">
+        <v>6763082.4631743049</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A178">
+        <v>115.33398072</v>
+      </c>
+      <c r="B178">
+        <v>-29.247859549999902</v>
+      </c>
+      <c r="C178">
+        <v>338106.45684481633</v>
+      </c>
+      <c r="D178">
+        <v>6763402.9621444549</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A179">
+        <v>115.33222429</v>
+      </c>
+      <c r="B179">
+        <v>-29.241994795999901</v>
+      </c>
+      <c r="C179">
+        <v>337926.50728217489</v>
+      </c>
+      <c r="D179">
+        <v>6764050.4681683164</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A180">
+        <v>115.331906734</v>
+      </c>
+      <c r="B180">
+        <v>-29.2403214099999</v>
+      </c>
+      <c r="C180">
+        <v>337893.00469174632</v>
+      </c>
+      <c r="D180">
+        <v>6764235.4740117984</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A181">
+        <v>115.331789732</v>
+      </c>
+      <c r="B181">
+        <v>-29.2388851689999</v>
+      </c>
+      <c r="C181">
+        <v>337879.36834790476</v>
+      </c>
+      <c r="D181">
+        <v>6764394.4766444536</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A182">
+        <v>115.331849859</v>
+      </c>
+      <c r="B182">
+        <v>-29.237261665999899</v>
+      </c>
+      <c r="C182">
+        <v>337882.65321373485</v>
+      </c>
+      <c r="D182">
+        <v>6764574.476547854</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A183">
+        <v>115.33201873100001</v>
+      </c>
+      <c r="B183">
+        <v>-29.236469782999901</v>
+      </c>
+      <c r="C183">
+        <v>337897.81914673897</v>
+      </c>
+      <c r="D183">
+        <v>6764662.4665537253</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A184">
+        <v>115.33220336700001</v>
+      </c>
+      <c r="B184">
+        <v>-29.236029854999899</v>
+      </c>
+      <c r="C184">
+        <v>337915.07228672487</v>
+      </c>
+      <c r="D184">
+        <v>6764711.474635059</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A185">
+        <v>115.332461493</v>
+      </c>
+      <c r="B185">
+        <v>-29.2356405969999</v>
+      </c>
+      <c r="C185">
+        <v>337939.54865301726</v>
+      </c>
+      <c r="D185">
+        <v>6764754.9689967837</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A186">
+        <v>115.332808547</v>
+      </c>
+      <c r="B186">
+        <v>-29.2352839059999</v>
+      </c>
+      <c r="C186">
+        <v>337972.72034329758</v>
+      </c>
+      <c r="D186">
+        <v>6764794.9770976454</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A187">
+        <v>115.33352062</v>
+      </c>
+      <c r="B187">
+        <v>-29.234755911999901</v>
+      </c>
+      <c r="C187">
+        <v>338041.10257076041</v>
+      </c>
+      <c r="D187">
+        <v>6764854.4730856363</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A188">
+        <v>115.334214738</v>
+      </c>
+      <c r="B188">
+        <v>-29.234344967999899</v>
+      </c>
+      <c r="C188">
+        <v>338107.92449665978</v>
+      </c>
+      <c r="D188">
+        <v>6764900.9723609686</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A189">
+        <v>115.350418268</v>
+      </c>
+      <c r="B189">
+        <v>-29.230738240999901</v>
+      </c>
+      <c r="C189">
+        <v>339677.3001913738</v>
+      </c>
+      <c r="D189">
+        <v>6765322.9287487641</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A190">
+        <v>115.351125702</v>
+      </c>
+      <c r="B190">
+        <v>-29.230516679999901</v>
+      </c>
+      <c r="C190">
+        <v>339745.72049345885</v>
+      </c>
+      <c r="D190">
+        <v>6765348.4488635994</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A191">
+        <v>115.352147702</v>
+      </c>
+      <c r="B191">
+        <v>-29.230087058999899</v>
+      </c>
+      <c r="C191">
+        <v>339844.39438211126</v>
+      </c>
+      <c r="D191">
+        <v>6765397.4552310836</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A192">
+        <v>115.353749322</v>
+      </c>
+      <c r="B192">
+        <v>-29.229136742999899</v>
+      </c>
+      <c r="C192">
+        <v>339998.60123106395</v>
+      </c>
+      <c r="D192">
+        <v>6765504.9546306571</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A193">
+        <v>115.364363521</v>
+      </c>
+      <c r="B193">
+        <v>-29.221488489999899</v>
+      </c>
+      <c r="C193">
+        <v>341018.54143964447</v>
+      </c>
+      <c r="D193">
+        <v>6766366.9590551071</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A194">
+        <v>115.37000076299999</v>
+      </c>
+      <c r="B194">
+        <v>-29.2176498769999</v>
+      </c>
+      <c r="C194">
+        <v>341560.64190014731</v>
+      </c>
+      <c r="D194">
+        <v>6766799.9753571171</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A195">
+        <v>115.375020636</v>
+      </c>
+      <c r="B195">
+        <v>-29.2143721109999</v>
+      </c>
+      <c r="C195">
+        <v>342043.62348225102</v>
+      </c>
+      <c r="D195">
+        <v>6767169.9807358477</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A196">
+        <v>115.379782342</v>
+      </c>
+      <c r="B196">
+        <v>-29.2115242459999</v>
+      </c>
+      <c r="C196">
+        <v>342502.19421701459</v>
+      </c>
+      <c r="D196">
+        <v>6767491.9767576419</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A197">
+        <v>115.3825238</v>
+      </c>
+      <c r="B197">
+        <v>-29.210054868999901</v>
+      </c>
+      <c r="C197">
+        <v>342766.47873979609</v>
+      </c>
+      <c r="D197">
+        <v>6767658.4866388086</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A198">
+        <v>115.38568925</v>
+      </c>
+      <c r="B198">
+        <v>-29.208459807999901</v>
+      </c>
+      <c r="C198">
+        <v>343071.80148408952</v>
+      </c>
+      <c r="D198">
+        <v>6767839.4850796014</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A199">
+        <v>115.390782851</v>
+      </c>
+      <c r="B199">
+        <v>-29.206044190999901</v>
+      </c>
+      <c r="C199">
+        <v>343563.35278066655</v>
+      </c>
+      <c r="D199">
+        <v>6768113.9786217837</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A200">
+        <v>115.39683589099999</v>
+      </c>
+      <c r="B200">
+        <v>-29.203382641999902</v>
+      </c>
+      <c r="C200">
+        <v>344147.8396225248</v>
+      </c>
+      <c r="D200">
+        <v>6768416.9777253428</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A201">
+        <v>115.401739451</v>
+      </c>
+      <c r="B201">
+        <v>-29.201365769999899</v>
+      </c>
+      <c r="C201">
+        <v>344621.56362173765</v>
+      </c>
+      <c r="D201">
+        <v>6768646.9830558803</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A202">
+        <v>115.408073268</v>
+      </c>
+      <c r="B202">
+        <v>-29.198941644999898</v>
+      </c>
+      <c r="C202">
+        <v>345233.76117574517</v>
+      </c>
+      <c r="D202">
+        <v>6768923.9848411866</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A203">
+        <v>115.41227665</v>
+      </c>
+      <c r="B203">
+        <v>-29.197475524999899</v>
+      </c>
+      <c r="C203">
+        <v>345640.27003643342</v>
+      </c>
+      <c r="D203">
+        <v>6769091.989987392</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A204">
+        <v>115.41706177899999</v>
+      </c>
+      <c r="B204">
+        <v>-29.195993654999899</v>
+      </c>
+      <c r="C204">
+        <v>346103.33296522719</v>
+      </c>
+      <c r="D204">
+        <v>6769262.488135268</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A205">
+        <v>115.421081907</v>
+      </c>
+      <c r="B205">
+        <v>-29.194926711999901</v>
+      </c>
+      <c r="C205">
+        <v>346492.6410296922</v>
+      </c>
+      <c r="D205">
+        <v>6769385.9860694706</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A206">
+        <v>115.424610954</v>
+      </c>
+      <c r="B206">
+        <v>-29.1941516599999</v>
+      </c>
+      <c r="C206">
+        <v>346834.63951473858</v>
+      </c>
+      <c r="D206">
+        <v>6769476.483460282</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A207">
+        <v>115.42798450700001</v>
+      </c>
+      <c r="B207">
+        <v>-29.193582224999901</v>
+      </c>
+      <c r="C207">
+        <v>347161.82806360803</v>
+      </c>
+      <c r="D207">
+        <v>6769543.9821965843</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A208">
+        <v>115.431510003</v>
+      </c>
+      <c r="B208">
+        <v>-29.193158854999901</v>
+      </c>
+      <c r="C208">
+        <v>347504.01074353035</v>
+      </c>
+      <c r="D208">
+        <v>6769595.4823051179</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A209">
+        <v>115.435424654</v>
+      </c>
+      <c r="B209">
+        <v>-29.1928888069999</v>
+      </c>
+      <c r="C209">
+        <v>347884.26289478096</v>
+      </c>
+      <c r="D209">
+        <v>6769630.4856161932</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A210">
+        <v>115.438624734</v>
+      </c>
+      <c r="B210">
+        <v>-29.1927953759999</v>
+      </c>
+      <c r="C210">
+        <v>348195.29352421011</v>
+      </c>
+      <c r="D210">
+        <v>6769644.980549668</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A211">
+        <v>115.44273813700001</v>
+      </c>
+      <c r="B211">
+        <v>-29.192789204999901</v>
+      </c>
+      <c r="C211">
+        <v>348595.2621236238</v>
+      </c>
+      <c r="D211">
+        <v>6769650.9751118068</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A212">
+        <v>115.44657857</v>
+      </c>
+      <c r="B212">
+        <v>-29.1929420919999</v>
+      </c>
+      <c r="C212">
+        <v>348968.92058035254</v>
+      </c>
+      <c r="D212">
+        <v>6769638.9783999659</v>
+      </c>
+    </row>
+    <row r="213" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A213">
+        <v>115.448722761</v>
+      </c>
+      <c r="B213">
+        <v>-29.1932196489999</v>
+      </c>
+      <c r="C213">
+        <v>349177.82231158839</v>
+      </c>
+      <c r="D213">
+        <v>6769610.9765632823</v>
+      </c>
+    </row>
+    <row r="214" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A214">
+        <v>115.450823317</v>
+      </c>
+      <c r="B214">
+        <v>-29.193686150999898</v>
+      </c>
+      <c r="C214">
+        <v>349382.75609013555</v>
+      </c>
+      <c r="D214">
+        <v>6769561.9768467098</v>
+      </c>
+    </row>
+    <row r="215" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A215">
+        <v>115.453085938</v>
+      </c>
+      <c r="B215">
+        <v>-29.1943124689999</v>
+      </c>
+      <c r="C215">
+        <v>349603.67977182689</v>
+      </c>
+      <c r="D215">
+        <v>6769495.4709495027</v>
+      </c>
+    </row>
+    <row r="216" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A216">
+        <v>115.45516742300001</v>
+      </c>
+      <c r="B216">
+        <v>-29.194999720999899</v>
+      </c>
+      <c r="C216">
+        <v>349807.07669026731</v>
+      </c>
+      <c r="D216">
+        <v>6769421.9767417395</v>
+      </c>
+    </row>
+    <row r="217" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A217">
+        <v>115.456592663</v>
+      </c>
+      <c r="B217">
+        <v>-29.195598213999901</v>
+      </c>
+      <c r="C217">
+        <v>349946.53187346191</v>
+      </c>
+      <c r="D217">
+        <v>6769357.4764396045</v>
+      </c>
+    </row>
+    <row r="218" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A218">
+        <v>115.458226727</v>
+      </c>
+      <c r="B218">
+        <v>-29.196447277999901</v>
+      </c>
+      <c r="C218">
+        <v>350106.65478052507</v>
+      </c>
+      <c r="D218">
+        <v>6769265.4738650154</v>
+      </c>
+    </row>
+    <row r="219" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A219">
+        <v>115.461261522</v>
+      </c>
+      <c r="B219">
+        <v>-29.198264450999901</v>
+      </c>
+      <c r="C219">
+        <v>350404.37805414828</v>
+      </c>
+      <c r="D219">
+        <v>6769067.9729227237</v>
+      </c>
+    </row>
+    <row r="220" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A220">
+        <v>115.465996565</v>
+      </c>
+      <c r="B220">
+        <v>-29.2012832039999</v>
+      </c>
+      <c r="C220">
+        <v>350869.14593193564</v>
+      </c>
+      <c r="D220">
+        <v>6768739.4716773257</v>
+      </c>
+    </row>
+    <row r="221" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A221">
+        <v>115.47318323499999</v>
+      </c>
+      <c r="B221">
+        <v>-29.206328568999901</v>
+      </c>
+      <c r="C221">
+        <v>351575.16948042717</v>
+      </c>
+      <c r="D221">
+        <v>6768189.4747614488</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{701263F8-3BED-4833-888B-23EA6272BAEC}">
   <dimension ref="A1:E225"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A207" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:E225"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -24994,12 +28104,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22F5D9FE-7C49-48B3-9367-2F5352B6C0CB}">
   <dimension ref="A1:E400"/>
   <sheetViews>
-    <sheetView topLeftCell="A382" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:E400"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G222" sqref="G222"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
shapefile updates and spatial updates
</commit_message>
<xml_diff>
--- a/Data/Data_geology/Otorowiri_outcrop.xlsx
+++ b/Data/Data_geology/Otorowiri_outcrop.xlsx
@@ -8,18 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\00105010\Projects\Otorowiri\data\data_geology\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9966DA22-6EDC-4940-B65C-745017A8DD0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFD155C4-F636-4286-BB26-C6BE2926A8CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="4" xr2:uid="{3885F5B0-7C21-4634-A104-1A3CDF95EC0E}"/>
+    <workbookView xWindow="40020" yWindow="-16455" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="4" xr2:uid="{3885F5B0-7C21-4634-A104-1A3CDF95EC0E}"/>
   </bookViews>
   <sheets>
     <sheet name="Otorowiri_1" sheetId="1" r:id="rId1"/>
     <sheet name="Otorowiri_2" sheetId="2" r:id="rId2"/>
     <sheet name="Otorowiri_3" sheetId="3" r:id="rId3"/>
     <sheet name="Otorowiri-Parmelia contact" sheetId="4" r:id="rId4"/>
-    <sheet name="Yarragadee-Otorowiri contact" sheetId="7" r:id="rId5"/>
-    <sheet name="Yarragadee-Otorowiri_NEW" sheetId="6" r:id="rId6"/>
-    <sheet name="Otorowiri-Parmelia_NEW" sheetId="5" r:id="rId7"/>
+    <sheet name="O-P contact simplified" sheetId="9" r:id="rId5"/>
+    <sheet name="Yarragadee-Otorowiri contact" sheetId="7" r:id="rId6"/>
+    <sheet name="Y-O contact simplified" sheetId="8" r:id="rId7"/>
+    <sheet name="Yarragadee-Otorowiri_NEW" sheetId="6" r:id="rId8"/>
+    <sheet name="Otorowiri-Parmelia_NEW" sheetId="5" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="629">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="629">
   <si>
     <t>Longitude</t>
   </si>
@@ -14727,7 +14729,7 @@
   <dimension ref="A1:D458"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="A1:D1"/>
+      <selection activeCell="C1" sqref="C1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -21153,10 +21155,929 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35B33FD7-38C7-497F-B8A4-85FBD6DAE9A7}">
+  <dimension ref="A1:B113"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>353021.99255767401</v>
+      </c>
+      <c r="B2">
+        <v>6765869.0254175104</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>352848.23874475801</v>
+      </c>
+      <c r="B3">
+        <v>6765928.7532906998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>352603.89744534402</v>
+      </c>
+      <c r="B4">
+        <v>6766048.2090370804</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>352522.45034553902</v>
+      </c>
+      <c r="B5">
+        <v>6766140.5157501996</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>352283.53885277902</v>
+      </c>
+      <c r="B6">
+        <v>6766292.5503364997</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>352066.34658663301</v>
+      </c>
+      <c r="B7">
+        <v>6766417.43588953</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>351876.30335375603</v>
+      </c>
+      <c r="B8">
+        <v>6766553.1810558699</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>351783.99664064398</v>
+      </c>
+      <c r="B9">
+        <v>6766623.7685423698</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>351512.506307962</v>
+      </c>
+      <c r="B10">
+        <v>6766786.6627419796</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>351322.46307508502</v>
+      </c>
+      <c r="B11">
+        <v>6766927.8377149701</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>351230.15636197297</v>
+      </c>
+      <c r="B12">
+        <v>6767079.8723012796</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>351078.12177567102</v>
+      </c>
+      <c r="B13">
+        <v>6767210.1876609595</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>350953.236222637</v>
+      </c>
+      <c r="B14">
+        <v>6767351.3626339603</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>350839.21028291102</v>
+      </c>
+      <c r="B15">
+        <v>6767552.2654801402</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>350795.77182968199</v>
+      </c>
+      <c r="B16">
+        <v>6767620.1380633097</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>350741.47376314498</v>
+      </c>
+      <c r="B17">
+        <v>6767698.8702597897</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>350657.31176001398</v>
+      </c>
+      <c r="B18">
+        <v>6767850.9048460899</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>350584.00937018998</v>
+      </c>
+      <c r="B19">
+        <v>6767962.2158824904</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>350505.27717371198</v>
+      </c>
+      <c r="B20">
+        <v>6768073.52691889</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>350426.54497723398</v>
+      </c>
+      <c r="B21">
+        <v>6768152.25911537</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>350317.94884416199</v>
+      </c>
+      <c r="B22">
+        <v>6768201.1273752498</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>350107.54383633297</v>
+      </c>
+      <c r="B23">
+        <v>6768243.2083768202</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>349989.44554161601</v>
+      </c>
+      <c r="B24">
+        <v>6768236.4211184997</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>349689.44872400298</v>
+      </c>
+      <c r="B25">
+        <v>6768115.6079204604</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>349635.15065746597</v>
+      </c>
+      <c r="B26">
+        <v>6768103.3908554902</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>349545.55884768098</v>
+      </c>
+      <c r="B27">
+        <v>6768095.2461455101</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>349374.51993809198</v>
+      </c>
+      <c r="B28">
+        <v>6768088.4588871896</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>349295.78774161398</v>
+      </c>
+      <c r="B29">
+        <v>6768088.4588871896</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>348786.743367836</v>
+      </c>
+      <c r="B30">
+        <v>6768133.2547920803</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A31">
+        <v>348612.98955491901</v>
+      </c>
+      <c r="B31">
+        <v>6768133.2547920803</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A32">
+        <v>348200.32424924301</v>
+      </c>
+      <c r="B32">
+        <v>6768182.1230519703</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A33">
+        <v>347809.37817018002</v>
+      </c>
+      <c r="B33">
+        <v>6768133.2547920803</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A34">
+        <v>347212.09943827998</v>
+      </c>
+      <c r="B34">
+        <v>6768062.6673055897</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A35">
+        <v>346674.54857957002</v>
+      </c>
+      <c r="B35">
+        <v>6767899.7731059799</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A36">
+        <v>346234.734240625</v>
+      </c>
+      <c r="B36">
+        <v>6767747.7385196798</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A37">
+        <v>345974.10352125001</v>
+      </c>
+      <c r="B37">
+        <v>6767622.8529666401</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A38">
+        <v>345441.98246919399</v>
+      </c>
+      <c r="B38">
+        <v>6767400.2308938401</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A39">
+        <v>344736.10760422098</v>
+      </c>
+      <c r="B39">
+        <v>6767090.7319145901</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A40">
+        <v>343943.35583278898</v>
+      </c>
+      <c r="B40">
+        <v>6766667.2069955999</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A41">
+        <v>343204.90212789399</v>
+      </c>
+      <c r="B41">
+        <v>6766254.5416899296</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A42">
+        <v>342737.93875568098</v>
+      </c>
+      <c r="B42">
+        <v>6765950.47251732</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A43">
+        <v>341825.73123787</v>
+      </c>
+      <c r="B43">
+        <v>6765114.2822926603</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A44">
+        <v>340489.99880107498</v>
+      </c>
+      <c r="B44">
+        <v>6763843.7075357102</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A45">
+        <v>340207.64885508502</v>
+      </c>
+      <c r="B45">
+        <v>6763561.3575897198</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A46">
+        <v>340229.3680817</v>
+      </c>
+      <c r="B46">
+        <v>6762529.69432553</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A47">
+        <v>340403.12189461599</v>
+      </c>
+      <c r="B47">
+        <v>6761671.7848742604</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A48">
+        <v>340576.87570753298</v>
+      </c>
+      <c r="B48">
+        <v>6760846.4542629002</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A49">
+        <v>340718.050680527</v>
+      </c>
+      <c r="B49">
+        <v>6760531.5254769903</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A50">
+        <v>340750.62952044897</v>
+      </c>
+      <c r="B50">
+        <v>6759966.8255850105</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A51">
+        <v>341315.32941242802</v>
+      </c>
+      <c r="B51">
+        <v>6758381.3220421504</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A52">
+        <v>341923.46775763499</v>
+      </c>
+      <c r="B52">
+        <v>6757447.3952977201</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A53">
+        <v>342118.94079716603</v>
+      </c>
+      <c r="B53">
+        <v>6756730.6608194401</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A54">
+        <v>342053.78311732301</v>
+      </c>
+      <c r="B54">
+        <v>6755992.2071145503</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A55">
+        <v>342162.379250395</v>
+      </c>
+      <c r="B55">
+        <v>6754862.8073305897</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A56">
+        <v>342292.69461008301</v>
+      </c>
+      <c r="B56">
+        <v>6753776.8459998602</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A57">
+        <v>342292.69461008301</v>
+      </c>
+      <c r="B57">
+        <v>6753125.2692014296</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A58">
+        <v>342379.57151654101</v>
+      </c>
+      <c r="B58">
+        <v>6752213.0616836101</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A59">
+        <v>342879.11372867599</v>
+      </c>
+      <c r="B59">
+        <v>6751279.13493919</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A60">
+        <v>343422.09439404</v>
+      </c>
+      <c r="B60">
+        <v>6750692.7158206003</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A61">
+        <v>344030.23273924697</v>
+      </c>
+      <c r="B61">
+        <v>6749910.8236624701</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A62">
+        <v>345702.61318856798</v>
+      </c>
+      <c r="B62">
+        <v>6748042.9701736197</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A63">
+        <v>346614.82070638001</v>
+      </c>
+      <c r="B63">
+        <v>6747261.0780154997</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A64">
+        <v>347092.64369190001</v>
+      </c>
+      <c r="B64">
+        <v>6746196.8359113801</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A65">
+        <v>347635.62435726402</v>
+      </c>
+      <c r="B65">
+        <v>6744546.1746886801</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A66">
+        <v>348070.008889555</v>
+      </c>
+      <c r="B66">
+        <v>6743243.0210918002</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A67">
+        <v>348678.14723476302</v>
+      </c>
+      <c r="B67">
+        <v>6741852.9905884704</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A68">
+        <v>349329.72403319902</v>
+      </c>
+      <c r="B68">
+        <v>6740636.7138980599</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A69">
+        <v>349677.231659032</v>
+      </c>
+      <c r="B69">
+        <v>6740289.2062722296</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A70">
+        <v>350589.43917684403</v>
+      </c>
+      <c r="B70">
+        <v>6739919.97941978</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A71">
+        <v>351458.20824142598</v>
+      </c>
+      <c r="B71">
+        <v>6739724.5063802497</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A72">
+        <v>352565.88879876799</v>
+      </c>
+      <c r="B72">
+        <v>6739659.3487004004</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A73">
+        <v>353217.46559720498</v>
+      </c>
+      <c r="B73">
+        <v>6739507.3141141003</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A74">
+        <v>353760.44626256899</v>
+      </c>
+      <c r="B74">
+        <v>6739224.9641681099</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A75">
+        <v>353651.85012949602</v>
+      </c>
+      <c r="B75">
+        <v>6738551.6681430601</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A76">
+        <v>353369.50018350699</v>
+      </c>
+      <c r="B76">
+        <v>6738052.1259309296</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A77">
+        <v>353065.43101090298</v>
+      </c>
+      <c r="B77">
+        <v>6737270.2337728003</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A78">
+        <v>352609.32725199801</v>
+      </c>
+      <c r="B78">
+        <v>6735597.8533234801</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A79">
+        <v>352240.10039954999</v>
+      </c>
+      <c r="B79">
+        <v>6733990.6305539999</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A80">
+        <v>352066.346586634</v>
+      </c>
+      <c r="B80">
+        <v>6733230.4576224899</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A81">
+        <v>351762.27741402999</v>
+      </c>
+      <c r="B81">
+        <v>6732296.5308780698</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A82">
+        <v>351783.99664064503</v>
+      </c>
+      <c r="B82">
+        <v>6731601.5156263998</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A83">
+        <v>351653.68128095701</v>
+      </c>
+      <c r="B83">
+        <v>6730819.6234682798</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A84">
+        <v>351219.29674866598</v>
+      </c>
+      <c r="B84">
+        <v>6730341.8004827602</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A85">
+        <v>350676.31608330202</v>
+      </c>
+      <c r="B85">
+        <v>6730146.3274432197</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A86">
+        <v>350307.089230855</v>
+      </c>
+      <c r="B86">
+        <v>6729929.1351770796</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A87">
+        <v>349546.91629934497</v>
+      </c>
+      <c r="B87">
+        <v>6729603.3467778601</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A88">
+        <v>349373.16248642898</v>
+      </c>
+      <c r="B88">
+        <v>6729342.7160584899</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A89">
+        <v>349177.689446898</v>
+      </c>
+      <c r="B89">
+        <v>6728712.8584866598</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A90">
+        <v>349003.93563398102</v>
+      </c>
+      <c r="B90">
+        <v>6727540.0202494804</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A91">
+        <v>348895.33950090897</v>
+      </c>
+      <c r="B91">
+        <v>6726562.65505182</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A92">
+        <v>348547.83187507599</v>
+      </c>
+      <c r="B92">
+        <v>6725541.8514009397</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A93">
+        <v>348287.20115570101</v>
+      </c>
+      <c r="B93">
+        <v>6723500.24409917</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A94">
+        <v>348222.043475857</v>
+      </c>
+      <c r="B94">
+        <v>6722327.4058619896</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A95">
+        <v>348070.008889555</v>
+      </c>
+      <c r="B95">
+        <v>6721719.2675167797</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A96">
+        <v>347831.097396795</v>
+      </c>
+      <c r="B96">
+        <v>6720372.6754666697</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A97">
+        <v>347722.50126372202</v>
+      </c>
+      <c r="B97">
+        <v>6719373.5910424097</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A98">
+        <v>347570.46667742101</v>
+      </c>
+      <c r="B98">
+        <v>6718787.1719238097</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A99">
+        <v>347374.99363788898</v>
+      </c>
+      <c r="B99">
+        <v>6715681.3225179296</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A100">
+        <v>347288.11673143099</v>
+      </c>
+      <c r="B100">
+        <v>6713813.4690290801</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A101">
+        <v>347374.99363788898</v>
+      </c>
+      <c r="B101">
+        <v>6711033.4080224102</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A102">
+        <v>347461.87054434803</v>
+      </c>
+      <c r="B102">
+        <v>6708123.0316560604</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A103">
+        <v>346984.04755882698</v>
+      </c>
+      <c r="B103">
+        <v>6705690.4782752302</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A104">
+        <v>346897.17065236898</v>
+      </c>
+      <c r="B104">
+        <v>6703952.94014607</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A105">
+        <v>347722.50126372202</v>
+      </c>
+      <c r="B105">
+        <v>6700152.0754885199</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A106">
+        <v>348439.23574200302</v>
+      </c>
+      <c r="B106">
+        <v>6699055.25454449</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A107">
+        <v>349753.248952183</v>
+      </c>
+      <c r="B107">
+        <v>6696959.3491761796</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A108">
+        <v>350795.77182968199</v>
+      </c>
+      <c r="B108">
+        <v>6693397.3960114</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A109">
+        <v>350969.52564259898</v>
+      </c>
+      <c r="B109">
+        <v>6690791.0888176505</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A110">
+        <v>351751.41780072299</v>
+      </c>
+      <c r="B110">
+        <v>6685665.3513366096</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A111">
+        <v>352185.80233301403</v>
+      </c>
+      <c r="B111">
+        <v>6682103.39817183</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A112">
+        <v>352533.30995884701</v>
+      </c>
+      <c r="B112">
+        <v>6679062.7064457899</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A113">
+        <v>353836.46355571999</v>
+      </c>
+      <c r="B113">
+        <v>6675761.3840003796</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1556757B-BEF5-4EA2-92E7-842579201367}">
   <dimension ref="A1:D221"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
@@ -24261,7 +25182,606 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82E3E11C-5152-4597-8929-70F654A7A7EA}">
+  <dimension ref="A1:B73"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>351604.81302107498</v>
+      </c>
+      <c r="B2">
+        <v>6768187.5528586302</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>350888.07854279398</v>
+      </c>
+      <c r="B3">
+        <v>6768708.8142973799</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>350225.64213105</v>
+      </c>
+      <c r="B4">
+        <v>6769186.6372828996</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>349780.39798545197</v>
+      </c>
+      <c r="B5">
+        <v>6769436.4083889704</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>349096.24234709301</v>
+      </c>
+      <c r="B6">
+        <v>6769631.8814284997</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>348249.19250912598</v>
+      </c>
+      <c r="B7">
+        <v>6769664.4602684202</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>347293.54653808498</v>
+      </c>
+      <c r="B8">
+        <v>6769599.3025885802</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>346555.09283318999</v>
+      </c>
+      <c r="B9">
+        <v>6769425.5487756599</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>345501.710342384</v>
+      </c>
+      <c r="B10">
+        <v>6769078.0411498304</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>344556.92398465099</v>
+      </c>
+      <c r="B11">
+        <v>6768632.7970042303</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>343568.699173689</v>
+      </c>
+      <c r="B12">
+        <v>6768154.9740187097</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>342710.78972241399</v>
+      </c>
+      <c r="B13">
+        <v>6767644.5721932696</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>341766.00336467999</v>
+      </c>
+      <c r="B14">
+        <v>6767014.7146214396</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>339811.27296937001</v>
+      </c>
+      <c r="B15">
+        <v>6765407.4918519696</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>339203.13462416298</v>
+      </c>
+      <c r="B16">
+        <v>6765212.0188124403</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>338334.36555957998</v>
+      </c>
+      <c r="B17">
+        <v>6764994.82654629</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>337921.70025390398</v>
+      </c>
+      <c r="B18">
+        <v>6764669.0381470704</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>337899.981027289</v>
+      </c>
+      <c r="B19">
+        <v>6763865.4267623303</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>338160.61174666398</v>
+      </c>
+      <c r="B20">
+        <v>6763083.5346042104</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>338138.892520049</v>
+      </c>
+      <c r="B21">
+        <v>6762366.8001259305</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>338073.73484020599</v>
+      </c>
+      <c r="B22">
+        <v>6761954.1348202499</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>338204.05019989301</v>
+      </c>
+      <c r="B23">
+        <v>6761237.4003419699</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>338681.87318541302</v>
+      </c>
+      <c r="B24">
+        <v>6760564.10431692</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>339290.01153062098</v>
+      </c>
+      <c r="B25">
+        <v>6759586.7391192699</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>339659.238383068</v>
+      </c>
+      <c r="B26">
+        <v>6758066.3932562498</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>340028.46523551602</v>
+      </c>
+      <c r="B27">
+        <v>6756155.1013141703</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>340180.49982181803</v>
+      </c>
+      <c r="B28">
+        <v>6754504.44009146</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>340571.44590087997</v>
+      </c>
+      <c r="B29">
+        <v>6752658.3058292205</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>340897.23430009797</v>
+      </c>
+      <c r="B30">
+        <v>6751159.6791928196</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A31">
+        <v>341179.584246087</v>
+      </c>
+      <c r="B31">
+        <v>6750334.3485814696</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A32">
+        <v>342569.61474941898</v>
+      </c>
+      <c r="B32">
+        <v>6749052.9142112099</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A33">
+        <v>344046.52215920901</v>
+      </c>
+      <c r="B33">
+        <v>6747402.2529884996</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A34">
+        <v>344871.85277056199</v>
+      </c>
+      <c r="B34">
+        <v>6746229.4147513099</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A35">
+        <v>345870.93719483202</v>
+      </c>
+      <c r="B35">
+        <v>6744535.3150753798</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A36">
+        <v>346479.07554003998</v>
+      </c>
+      <c r="B36">
+        <v>6742884.6538526705</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A37">
+        <v>347391.28305785102</v>
+      </c>
+      <c r="B37">
+        <v>6740582.4158315295</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A38">
+        <v>347695.35223045503</v>
+      </c>
+      <c r="B38">
+        <v>6739539.8929540301</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A39">
+        <v>349432.89035961899</v>
+      </c>
+      <c r="B39">
+        <v>6739279.2622346599</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A40">
+        <v>350779.482409722</v>
+      </c>
+      <c r="B40">
+        <v>6738888.3161555901</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A41">
+        <v>351561.37456784601</v>
+      </c>
+      <c r="B41">
+        <v>6738453.9316232996</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A42">
+        <v>351822.00528722099</v>
+      </c>
+      <c r="B42">
+        <v>6737498.2856522603</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A43">
+        <v>351517.93611461698</v>
+      </c>
+      <c r="B43">
+        <v>6735891.0628827801</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A44">
+        <v>351040.11312909698</v>
+      </c>
+      <c r="B44">
+        <v>6733979.7709406996</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A45">
+        <v>350475.41323711799</v>
+      </c>
+      <c r="B45">
+        <v>6732459.4250776796</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A46">
+        <v>349823.83643868199</v>
+      </c>
+      <c r="B46">
+        <v>6730939.0792146698</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A47">
+        <v>348824.75201441202</v>
+      </c>
+      <c r="B47">
+        <v>6730330.9408694599</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A48">
+        <v>348260.05212243402</v>
+      </c>
+      <c r="B48">
+        <v>6729418.7333516497</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A49">
+        <v>347738.790683684</v>
+      </c>
+      <c r="B49">
+        <v>6727854.9490353996</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A50">
+        <v>347304.40615139302</v>
+      </c>
+      <c r="B50">
+        <v>6725509.2725610305</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A51">
+        <v>346870.02161910199</v>
+      </c>
+      <c r="B51">
+        <v>6723337.3498995798</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A52">
+        <v>346696.26780618599</v>
+      </c>
+      <c r="B52">
+        <v>6721339.1810510401</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A53">
+        <v>346261.88327389403</v>
+      </c>
+      <c r="B53">
+        <v>6719384.4506557202</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A54">
+        <v>346348.76018035301</v>
+      </c>
+      <c r="B54">
+        <v>6717342.8433539597</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A55">
+        <v>346131.567914207</v>
+      </c>
+      <c r="B55">
+        <v>6714606.2208005199</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A56">
+        <v>346001.25255451998</v>
+      </c>
+      <c r="B56">
+        <v>6712217.1058729198</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A57">
+        <v>346044.691007749</v>
+      </c>
+      <c r="B57">
+        <v>6710566.4446502198</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A58">
+        <v>345936.09487467603</v>
+      </c>
+      <c r="B58">
+        <v>6708177.3297226103</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A59">
+        <v>345501.71034238499</v>
+      </c>
+      <c r="B59">
+        <v>6706743.8607660504</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A60">
+        <v>345241.07962301001</v>
+      </c>
+      <c r="B60">
+        <v>6705571.02252887</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A61">
+        <v>345327.956529469</v>
+      </c>
+      <c r="B61">
+        <v>6704007.2382126199</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A62">
+        <v>345718.902608531</v>
+      </c>
+      <c r="B62">
+        <v>6702095.9462705404</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A63">
+        <v>346717.98703279998</v>
+      </c>
+      <c r="B63">
+        <v>6699576.51598325</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A64">
+        <v>347499.879190924</v>
+      </c>
+      <c r="B64">
+        <v>6698360.2392928395</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A65">
+        <v>348325.20980227803</v>
+      </c>
+      <c r="B65">
+        <v>6696753.0165233603</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A66">
+        <v>348933.348147485</v>
+      </c>
+      <c r="B66">
+        <v>6694407.34004898</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A67">
+        <v>349237.41732008901</v>
+      </c>
+      <c r="B67">
+        <v>6691453.5252294103</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A68">
+        <v>349584.92494592199</v>
+      </c>
+      <c r="B68">
+        <v>6687500.62598556</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A69">
+        <v>350062.74793144199</v>
+      </c>
+      <c r="B69">
+        <v>6683678.0421013897</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A70">
+        <v>350497.13246373303</v>
+      </c>
+      <c r="B70">
+        <v>6679030.1276058797</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A71">
+        <v>350801.20163633698</v>
+      </c>
+      <c r="B71">
+        <v>6677640.0971025499</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A72">
+        <v>351235.58616862801</v>
+      </c>
+      <c r="B72">
+        <v>6676988.5203041099</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A73">
+        <v>351669.97070091998</v>
+      </c>
+      <c r="B73">
+        <v>6675294.4206281798</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{701263F8-3BED-4833-888B-23EA6272BAEC}">
   <dimension ref="A1:E225"/>
   <sheetViews>
@@ -28104,7 +29624,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22F5D9FE-7C49-48B3-9367-2F5352B6C0CB}">
   <dimension ref="A1:E400"/>
   <sheetViews>

</xml_diff>

<commit_message>
All woody vegetation data and updated shapefiles with Main script changes
</commit_message>
<xml_diff>
--- a/Data/Data_geology/Otorowiri_outcrop.xlsx
+++ b/Data/Data_geology/Otorowiri_outcrop.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\00105010\Projects\Otorowiri\data\data_geology\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFD155C4-F636-4286-BB26-C6BE2926A8CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6F30C7F-BEFE-4FAD-BDF5-E87C8DA6A1BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40020" yWindow="-16455" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="4" xr2:uid="{3885F5B0-7C21-4634-A104-1A3CDF95EC0E}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="4" activeTab="4" xr2:uid="{3885F5B0-7C21-4634-A104-1A3CDF95EC0E}"/>
   </bookViews>
   <sheets>
     <sheet name="Otorowiri_1" sheetId="1" r:id="rId1"/>
@@ -21156,10 +21156,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35B33FD7-38C7-497F-B8A4-85FBD6DAE9A7}">
-  <dimension ref="A1:B113"/>
+  <dimension ref="A1:B94"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="H65" sqref="H65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -21174,897 +21174,745 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2">
-        <v>353021.99255767401</v>
+        <v>351979.77915992</v>
       </c>
       <c r="B2">
-        <v>6765869.0254175104</v>
+        <v>6767510.1873401096</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3">
-        <v>352848.23874475801</v>
+        <v>351088.03023817798</v>
       </c>
       <c r="B3">
-        <v>6765928.7532906998</v>
+        <v>6767773.8348474</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4">
-        <v>352603.89744534402</v>
+        <v>350281.57903938601</v>
       </c>
       <c r="B4">
-        <v>6766048.2090370804</v>
+        <v>6768029.7280162498</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5">
-        <v>352522.45034553902</v>
+        <v>350056.70322433801</v>
       </c>
       <c r="B5">
-        <v>6766140.5157501996</v>
+        <v>6768052.9910316002</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6">
-        <v>352283.53885277902</v>
+        <v>349689.44872400298</v>
       </c>
       <c r="B6">
-        <v>6766292.5503364997</v>
+        <v>6768115.6079204604</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7">
-        <v>352066.34658663301</v>
+        <v>349635.15065746597</v>
       </c>
       <c r="B7">
-        <v>6766417.43588953</v>
+        <v>6768103.3908554902</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8">
-        <v>351876.30335375603</v>
+        <v>349545.55884768098</v>
       </c>
       <c r="B8">
-        <v>6766553.1810558699</v>
+        <v>6768095.2461455101</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9">
-        <v>351783.99664064398</v>
+        <v>349374.51993809198</v>
       </c>
       <c r="B9">
-        <v>6766623.7685423698</v>
+        <v>6768088.4588871896</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10">
-        <v>351512.506307962</v>
+        <v>349295.78774161398</v>
       </c>
       <c r="B10">
-        <v>6766786.6627419796</v>
+        <v>6768088.4588871896</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11">
-        <v>351322.46307508502</v>
+        <v>348786.743367836</v>
       </c>
       <c r="B11">
-        <v>6766927.8377149701</v>
+        <v>6768133.2547920803</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12">
-        <v>351230.15636197297</v>
+        <v>348612.98955491901</v>
       </c>
       <c r="B12">
-        <v>6767079.8723012796</v>
+        <v>6768133.2547920803</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13">
-        <v>351078.12177567102</v>
+        <v>348200.32424924301</v>
       </c>
       <c r="B13">
-        <v>6767210.1876609595</v>
+        <v>6768182.1230519703</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14">
-        <v>350953.236222637</v>
+        <v>347809.37817018002</v>
       </c>
       <c r="B14">
-        <v>6767351.3626339603</v>
+        <v>6768133.2547920803</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15">
-        <v>350839.21028291102</v>
+        <v>347212.09943827998</v>
       </c>
       <c r="B15">
-        <v>6767552.2654801402</v>
+        <v>6768062.6673055897</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16">
-        <v>350795.77182968199</v>
+        <v>346674.54857957002</v>
       </c>
       <c r="B16">
-        <v>6767620.1380633097</v>
+        <v>6767899.7731059799</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17">
-        <v>350741.47376314498</v>
+        <v>346234.734240625</v>
       </c>
       <c r="B17">
-        <v>6767698.8702597897</v>
+        <v>6767747.7385196798</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18">
-        <v>350657.31176001398</v>
+        <v>345974.10352125001</v>
       </c>
       <c r="B18">
-        <v>6767850.9048460899</v>
+        <v>6767622.8529666401</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19">
-        <v>350584.00937018998</v>
+        <v>345441.98246919399</v>
       </c>
       <c r="B19">
-        <v>6767962.2158824904</v>
+        <v>6767400.2308938401</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20">
-        <v>350505.27717371198</v>
+        <v>344736.10760422098</v>
       </c>
       <c r="B20">
-        <v>6768073.52691889</v>
+        <v>6767090.7319145901</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21">
-        <v>350426.54497723398</v>
+        <v>343943.35583278898</v>
       </c>
       <c r="B21">
-        <v>6768152.25911537</v>
+        <v>6766667.2069955999</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22">
-        <v>350317.94884416199</v>
+        <v>343204.90212789399</v>
       </c>
       <c r="B22">
-        <v>6768201.1273752498</v>
+        <v>6766254.5416899296</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23">
-        <v>350107.54383633297</v>
+        <v>342737.93875568098</v>
       </c>
       <c r="B23">
-        <v>6768243.2083768202</v>
+        <v>6765950.47251732</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24">
-        <v>349989.44554161601</v>
+        <v>341825.73123787</v>
       </c>
       <c r="B24">
-        <v>6768236.4211184997</v>
+        <v>6765114.2822926603</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25">
-        <v>349689.44872400298</v>
+        <v>340489.99880107498</v>
       </c>
       <c r="B25">
-        <v>6768115.6079204604</v>
+        <v>6763843.7075357102</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26">
-        <v>349635.15065746597</v>
+        <v>340207.64885508502</v>
       </c>
       <c r="B26">
-        <v>6768103.3908554902</v>
+        <v>6763561.3575897198</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27">
-        <v>349545.55884768098</v>
+        <v>340229.3680817</v>
       </c>
       <c r="B27">
-        <v>6768095.2461455101</v>
+        <v>6762529.69432553</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28">
-        <v>349374.51993809198</v>
+        <v>340403.12189461599</v>
       </c>
       <c r="B28">
-        <v>6768088.4588871896</v>
+        <v>6761671.7848742604</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29">
-        <v>349295.78774161398</v>
+        <v>340576.87570753298</v>
       </c>
       <c r="B29">
-        <v>6768088.4588871896</v>
+        <v>6760846.4542629002</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30">
-        <v>348786.743367836</v>
+        <v>340718.050680527</v>
       </c>
       <c r="B30">
-        <v>6768133.2547920803</v>
+        <v>6760531.5254769903</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31">
-        <v>348612.98955491901</v>
+        <v>340750.62952044897</v>
       </c>
       <c r="B31">
-        <v>6768133.2547920803</v>
+        <v>6759966.8255850105</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32">
-        <v>348200.32424924301</v>
+        <v>341315.32941242802</v>
       </c>
       <c r="B32">
-        <v>6768182.1230519703</v>
+        <v>6758381.3220421504</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33">
-        <v>347809.37817018002</v>
+        <v>341923.46775763499</v>
       </c>
       <c r="B33">
-        <v>6768133.2547920803</v>
+        <v>6757447.3952977201</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34">
-        <v>347212.09943827998</v>
+        <v>342118.94079716603</v>
       </c>
       <c r="B34">
-        <v>6768062.6673055897</v>
+        <v>6756730.6608194401</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35">
-        <v>346674.54857957002</v>
+        <v>342053.78311732301</v>
       </c>
       <c r="B35">
-        <v>6767899.7731059799</v>
+        <v>6755992.2071145503</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36">
-        <v>346234.734240625</v>
+        <v>342162.379250395</v>
       </c>
       <c r="B36">
-        <v>6767747.7385196798</v>
+        <v>6754862.8073305897</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37">
-        <v>345974.10352125001</v>
+        <v>342292.69461008301</v>
       </c>
       <c r="B37">
-        <v>6767622.8529666401</v>
+        <v>6753776.8459998602</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38">
-        <v>345441.98246919399</v>
+        <v>342292.69461008301</v>
       </c>
       <c r="B38">
-        <v>6767400.2308938401</v>
+        <v>6753125.2692014296</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39">
-        <v>344736.10760422098</v>
+        <v>342379.57151654101</v>
       </c>
       <c r="B39">
-        <v>6767090.7319145901</v>
+        <v>6752213.0616836101</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40">
-        <v>343943.35583278898</v>
+        <v>342879.11372867599</v>
       </c>
       <c r="B40">
-        <v>6766667.2069955999</v>
+        <v>6751279.13493919</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41">
-        <v>343204.90212789399</v>
+        <v>343422.09439404</v>
       </c>
       <c r="B41">
-        <v>6766254.5416899296</v>
+        <v>6750692.7158206003</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42">
-        <v>342737.93875568098</v>
+        <v>344030.23273924697</v>
       </c>
       <c r="B42">
-        <v>6765950.47251732</v>
+        <v>6749910.8236624701</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43">
-        <v>341825.73123787</v>
+        <v>345702.61318856798</v>
       </c>
       <c r="B43">
-        <v>6765114.2822926603</v>
+        <v>6748042.9701736197</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44">
-        <v>340489.99880107498</v>
+        <v>346614.82070638001</v>
       </c>
       <c r="B44">
-        <v>6763843.7075357102</v>
+        <v>6747261.0780154997</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45">
-        <v>340207.64885508502</v>
+        <v>347092.64369190001</v>
       </c>
       <c r="B45">
-        <v>6763561.3575897198</v>
+        <v>6746196.8359113801</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46">
-        <v>340229.3680817</v>
+        <v>347635.62435726402</v>
       </c>
       <c r="B46">
-        <v>6762529.69432553</v>
+        <v>6744546.1746886801</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47">
-        <v>340403.12189461599</v>
+        <v>348070.008889555</v>
       </c>
       <c r="B47">
-        <v>6761671.7848742604</v>
+        <v>6743243.0210918002</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48">
-        <v>340576.87570753298</v>
+        <v>348678.14723476302</v>
       </c>
       <c r="B48">
-        <v>6760846.4542629002</v>
+        <v>6741852.9905884704</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49">
-        <v>340718.050680527</v>
+        <v>349329.72403319902</v>
       </c>
       <c r="B49">
-        <v>6760531.5254769903</v>
+        <v>6740636.7138980599</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50">
-        <v>340750.62952044897</v>
+        <v>349677.231659032</v>
       </c>
       <c r="B50">
-        <v>6759966.8255850105</v>
+        <v>6740289.2062722296</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51">
-        <v>341315.32941242802</v>
+        <v>350589.43917684403</v>
       </c>
       <c r="B51">
-        <v>6758381.3220421504</v>
+        <v>6739919.97941978</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52">
-        <v>341923.46775763499</v>
+        <v>351458.20824142598</v>
       </c>
       <c r="B52">
-        <v>6757447.3952977201</v>
+        <v>6739724.5063802497</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53">
-        <v>342118.94079716603</v>
+        <v>352565.88879876799</v>
       </c>
       <c r="B53">
-        <v>6756730.6608194401</v>
+        <v>6739659.3487004004</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54">
-        <v>342053.78311732301</v>
+        <v>353217.46559720498</v>
       </c>
       <c r="B54">
-        <v>6755992.2071145503</v>
+        <v>6739507.3141141003</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55">
-        <v>342162.379250395</v>
+        <v>353760.44626256899</v>
       </c>
       <c r="B55">
-        <v>6754862.8073305897</v>
+        <v>6739224.9641681099</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56">
-        <v>342292.69461008301</v>
+        <v>353651.85012949602</v>
       </c>
       <c r="B56">
-        <v>6753776.8459998602</v>
+        <v>6738551.6681430601</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57">
-        <v>342292.69461008301</v>
+        <v>353369.50018350699</v>
       </c>
       <c r="B57">
-        <v>6753125.2692014296</v>
+        <v>6738052.1259309296</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58">
-        <v>342379.57151654101</v>
+        <v>353065.43101090298</v>
       </c>
       <c r="B58">
-        <v>6752213.0616836101</v>
+        <v>6737270.2337728003</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59">
-        <v>342879.11372867599</v>
+        <v>352609.32725199801</v>
       </c>
       <c r="B59">
-        <v>6751279.13493919</v>
+        <v>6735597.8533234801</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60">
-        <v>343422.09439404</v>
+        <v>352240.10039954999</v>
       </c>
       <c r="B60">
-        <v>6750692.7158206003</v>
+        <v>6733990.6305539999</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61">
-        <v>344030.23273924697</v>
+        <v>352066.346586634</v>
       </c>
       <c r="B61">
-        <v>6749910.8236624701</v>
+        <v>6733230.4576224899</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62">
-        <v>345702.61318856798</v>
+        <v>351762.27741402999</v>
       </c>
       <c r="B62">
-        <v>6748042.9701736197</v>
+        <v>6732296.5308780698</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63">
-        <v>346614.82070638001</v>
+        <v>351783.99664064503</v>
       </c>
       <c r="B63">
-        <v>6747261.0780154997</v>
+        <v>6731601.5156263998</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64">
-        <v>347092.64369190001</v>
+        <v>351653.68128095701</v>
       </c>
       <c r="B64">
-        <v>6746196.8359113801</v>
+        <v>6730819.6234682798</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65">
-        <v>347635.62435726402</v>
+        <v>351219.29674866598</v>
       </c>
       <c r="B65">
-        <v>6744546.1746886801</v>
+        <v>6730341.8004827602</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66">
-        <v>348070.008889555</v>
+        <v>350676.31608330202</v>
       </c>
       <c r="B66">
-        <v>6743243.0210918002</v>
+        <v>6730146.3274432197</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67">
-        <v>348678.14723476302</v>
+        <v>350307.089230855</v>
       </c>
       <c r="B67">
-        <v>6741852.9905884704</v>
+        <v>6729929.1351770796</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68">
-        <v>349329.72403319902</v>
+        <v>349546.91629934497</v>
       </c>
       <c r="B68">
-        <v>6740636.7138980599</v>
+        <v>6729603.3467778601</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69">
-        <v>349677.231659032</v>
+        <v>349373.16248642898</v>
       </c>
       <c r="B69">
-        <v>6740289.2062722296</v>
+        <v>6729342.7160584899</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70">
-        <v>350589.43917684403</v>
+        <v>349177.689446898</v>
       </c>
       <c r="B70">
-        <v>6739919.97941978</v>
+        <v>6728712.8584866598</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71">
-        <v>351458.20824142598</v>
+        <v>349003.93563398102</v>
       </c>
       <c r="B71">
-        <v>6739724.5063802497</v>
+        <v>6727540.0202494804</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72">
-        <v>352565.88879876799</v>
+        <v>348895.33950090897</v>
       </c>
       <c r="B72">
-        <v>6739659.3487004004</v>
+        <v>6726562.65505182</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A73">
-        <v>353217.46559720498</v>
+        <v>348547.83187507599</v>
       </c>
       <c r="B73">
-        <v>6739507.3141141003</v>
+        <v>6725541.8514009397</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A74">
-        <v>353760.44626256899</v>
+        <v>348287.20115570101</v>
       </c>
       <c r="B74">
-        <v>6739224.9641681099</v>
+        <v>6723500.24409917</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A75">
-        <v>353651.85012949602</v>
+        <v>348222.043475857</v>
       </c>
       <c r="B75">
-        <v>6738551.6681430601</v>
+        <v>6722327.4058619896</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A76">
-        <v>353369.50018350699</v>
+        <v>348070.008889555</v>
       </c>
       <c r="B76">
-        <v>6738052.1259309296</v>
+        <v>6721719.2675167797</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A77">
-        <v>353065.43101090298</v>
+        <v>347831.097396795</v>
       </c>
       <c r="B77">
-        <v>6737270.2337728003</v>
+        <v>6720372.6754666697</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A78">
-        <v>352609.32725199801</v>
+        <v>347722.50126372202</v>
       </c>
       <c r="B78">
-        <v>6735597.8533234801</v>
+        <v>6719373.5910424097</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A79">
-        <v>352240.10039954999</v>
+        <v>347570.46667742101</v>
       </c>
       <c r="B79">
-        <v>6733990.6305539999</v>
+        <v>6718787.1719238097</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A80">
-        <v>352066.346586634</v>
+        <v>347374.99363788898</v>
       </c>
       <c r="B80">
-        <v>6733230.4576224899</v>
+        <v>6715681.3225179296</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A81">
-        <v>351762.27741402999</v>
+        <v>347288.11673143099</v>
       </c>
       <c r="B81">
-        <v>6732296.5308780698</v>
+        <v>6713813.4690290801</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A82">
-        <v>351783.99664064503</v>
+        <v>347374.99363788898</v>
       </c>
       <c r="B82">
-        <v>6731601.5156263998</v>
+        <v>6711033.4080224102</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A83">
-        <v>351653.68128095701</v>
+        <v>347461.87054434803</v>
       </c>
       <c r="B83">
-        <v>6730819.6234682798</v>
+        <v>6708123.0316560604</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84">
-        <v>351219.29674866598</v>
+        <v>346984.04755882698</v>
       </c>
       <c r="B84">
-        <v>6730341.8004827602</v>
+        <v>6705690.4782752302</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A85">
-        <v>350676.31608330202</v>
+        <v>346897.17065236898</v>
       </c>
       <c r="B85">
-        <v>6730146.3274432197</v>
+        <v>6703952.94014607</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A86">
-        <v>350307.089230855</v>
+        <v>347722.50126372202</v>
       </c>
       <c r="B86">
-        <v>6729929.1351770796</v>
+        <v>6700152.0754885199</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A87">
-        <v>349546.91629934497</v>
+        <v>348439.23574200302</v>
       </c>
       <c r="B87">
-        <v>6729603.3467778601</v>
+        <v>6699055.25454449</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A88">
-        <v>349373.16248642898</v>
+        <v>349753.248952183</v>
       </c>
       <c r="B88">
-        <v>6729342.7160584899</v>
+        <v>6696959.3491761796</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A89">
-        <v>349177.689446898</v>
+        <v>350795.77182968199</v>
       </c>
       <c r="B89">
-        <v>6728712.8584866598</v>
+        <v>6693397.3960114</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A90">
-        <v>349003.93563398102</v>
+        <v>350969.52564259898</v>
       </c>
       <c r="B90">
-        <v>6727540.0202494804</v>
+        <v>6690791.0888176505</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A91">
-        <v>348895.33950090897</v>
+        <v>351751.41780072299</v>
       </c>
       <c r="B91">
-        <v>6726562.65505182</v>
+        <v>6685665.3513366096</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A92">
-        <v>348547.83187507599</v>
+        <v>352185.80233301403</v>
       </c>
       <c r="B92">
-        <v>6725541.8514009397</v>
+        <v>6682103.39817183</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A93">
-        <v>348287.20115570101</v>
+        <v>352533.30995884701</v>
       </c>
       <c r="B93">
-        <v>6723500.24409917</v>
+        <v>6679062.7064457899</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A94">
-        <v>348222.043475857</v>
+        <v>353836.46355571999</v>
       </c>
       <c r="B94">
-        <v>6722327.4058619896</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A95">
-        <v>348070.008889555</v>
-      </c>
-      <c r="B95">
-        <v>6721719.2675167797</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A96">
-        <v>347831.097396795</v>
-      </c>
-      <c r="B96">
-        <v>6720372.6754666697</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A97">
-        <v>347722.50126372202</v>
-      </c>
-      <c r="B97">
-        <v>6719373.5910424097</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A98">
-        <v>347570.46667742101</v>
-      </c>
-      <c r="B98">
-        <v>6718787.1719238097</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A99">
-        <v>347374.99363788898</v>
-      </c>
-      <c r="B99">
-        <v>6715681.3225179296</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A100">
-        <v>347288.11673143099</v>
-      </c>
-      <c r="B100">
-        <v>6713813.4690290801</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A101">
-        <v>347374.99363788898</v>
-      </c>
-      <c r="B101">
-        <v>6711033.4080224102</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A102">
-        <v>347461.87054434803</v>
-      </c>
-      <c r="B102">
-        <v>6708123.0316560604</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A103">
-        <v>346984.04755882698</v>
-      </c>
-      <c r="B103">
-        <v>6705690.4782752302</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A104">
-        <v>346897.17065236898</v>
-      </c>
-      <c r="B104">
-        <v>6703952.94014607</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A105">
-        <v>347722.50126372202</v>
-      </c>
-      <c r="B105">
-        <v>6700152.0754885199</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A106">
-        <v>348439.23574200302</v>
-      </c>
-      <c r="B106">
-        <v>6699055.25454449</v>
-      </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A107">
-        <v>349753.248952183</v>
-      </c>
-      <c r="B107">
-        <v>6696959.3491761796</v>
-      </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A108">
-        <v>350795.77182968199</v>
-      </c>
-      <c r="B108">
-        <v>6693397.3960114</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A109">
-        <v>350969.52564259898</v>
-      </c>
-      <c r="B109">
-        <v>6690791.0888176505</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A110">
-        <v>351751.41780072299</v>
-      </c>
-      <c r="B110">
-        <v>6685665.3513366096</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A111">
-        <v>352185.80233301403</v>
-      </c>
-      <c r="B111">
-        <v>6682103.39817183</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A112">
-        <v>352533.30995884701</v>
-      </c>
-      <c r="B112">
-        <v>6679062.7064457899</v>
-      </c>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A113">
-        <v>353836.46355571999</v>
-      </c>
-      <c r="B113">
         <v>6675761.3840003796</v>
       </c>
     </row>
@@ -25186,8 +25034,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82E3E11C-5152-4597-8929-70F654A7A7EA}">
   <dimension ref="A1:B73"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -25202,42 +25050,42 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2">
-        <v>351604.81302107498</v>
+        <v>350991.10100755398</v>
       </c>
       <c r="B2">
-        <v>6768187.5528586302</v>
+        <v>6769049.4235224202</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3">
-        <v>350888.07854279398</v>
+        <v>350750.71651560598</v>
       </c>
       <c r="B3">
-        <v>6768708.8142973799</v>
+        <v>6769181.2472760696</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4">
-        <v>350225.64213105</v>
+        <v>350471.56033140898</v>
       </c>
       <c r="B4">
-        <v>6769186.6372828996</v>
+        <v>6769274.2993374597</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5">
-        <v>349780.39798545197</v>
+        <v>350052.82605511299</v>
       </c>
       <c r="B5">
-        <v>6769436.4083889704</v>
+        <v>6769367.3513988601</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6">
-        <v>349096.24234709301</v>
+        <v>349300.65522547002</v>
       </c>
       <c r="B6">
-        <v>6769631.8814284997</v>
+        <v>6769561.2098601097</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>